<commit_message>
egg grading considering number of eggs
</commit_message>
<xml_diff>
--- a/bovan_brown_max.xlsx
+++ b/bovan_brown_max.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="102" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="122" uniqueCount="38">
   <si>
     <t xml:space="preserve">Weeks</t>
   </si>
@@ -77,6 +77,18 @@
   </si>
   <si>
     <t xml:space="preserve">Week 18</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Week 19</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Week 20</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Week 21</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Week 22</t>
   </si>
   <si>
     <t xml:space="preserve">ID</t>
@@ -331,10 +343,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:CC10"/>
+  <dimension ref="A1:CS10"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="AW1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="CC3" activeCellId="0" sqref="CC3"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="BR1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="CR3" activeCellId="0" sqref="CR3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -383,6 +395,14 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="77" min="75" style="1" width="7.18"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="78" min="78" style="1" width="7.3"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="81" min="79" style="1" width="7.18"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="82" min="82" style="1" width="7.3"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="85" min="83" style="1" width="7.18"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="86" min="86" style="1" width="7.3"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="89" min="87" style="1" width="7.18"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="90" min="90" style="1" width="7.3"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="93" min="91" style="1" width="7.18"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="94" min="94" style="1" width="7.3"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="97" min="95" style="1" width="7.18"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="29.85" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -505,258 +525,330 @@
       <c r="CA1" s="3"/>
       <c r="CB1" s="3"/>
       <c r="CC1" s="3"/>
+      <c r="CD1" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="CE1" s="3"/>
+      <c r="CF1" s="3"/>
+      <c r="CG1" s="3"/>
+      <c r="CH1" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="CI1" s="3"/>
+      <c r="CJ1" s="3"/>
+      <c r="CK1" s="3"/>
+      <c r="CL1" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="CM1" s="3"/>
+      <c r="CN1" s="3"/>
+      <c r="CO1" s="3"/>
+      <c r="CP1" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="CQ1" s="3"/>
+      <c r="CR1" s="3"/>
+      <c r="CS1" s="3"/>
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="4" t="s">
-        <v>19</v>
+        <v>23</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>20</v>
+        <v>24</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>21</v>
+        <v>25</v>
       </c>
       <c r="D2" s="4" t="s">
-        <v>22</v>
+        <v>26</v>
       </c>
       <c r="E2" s="4" t="s">
-        <v>23</v>
+        <v>27</v>
       </c>
       <c r="F2" s="4" t="s">
-        <v>24</v>
+        <v>28</v>
       </c>
       <c r="G2" s="4" t="s">
-        <v>25</v>
+        <v>29</v>
       </c>
       <c r="H2" s="4" t="s">
-        <v>26</v>
+        <v>30</v>
       </c>
       <c r="I2" s="4" t="s">
-        <v>27</v>
+        <v>31</v>
       </c>
       <c r="J2" s="4" t="s">
-        <v>28</v>
+        <v>32</v>
       </c>
       <c r="K2" s="4" t="s">
-        <v>29</v>
+        <v>33</v>
       </c>
       <c r="L2" s="4" t="s">
-        <v>30</v>
+        <v>34</v>
       </c>
       <c r="M2" s="4" t="s">
-        <v>31</v>
+        <v>35</v>
       </c>
       <c r="N2" s="4" t="s">
-        <v>28</v>
+        <v>32</v>
       </c>
       <c r="O2" s="4" t="s">
-        <v>29</v>
+        <v>33</v>
       </c>
       <c r="P2" s="4" t="s">
-        <v>30</v>
+        <v>34</v>
       </c>
       <c r="Q2" s="4" t="s">
-        <v>31</v>
+        <v>35</v>
       </c>
       <c r="R2" s="4" t="s">
-        <v>28</v>
+        <v>32</v>
       </c>
       <c r="S2" s="4" t="s">
-        <v>29</v>
+        <v>33</v>
       </c>
       <c r="T2" s="4" t="s">
-        <v>30</v>
+        <v>34</v>
       </c>
       <c r="U2" s="4" t="s">
-        <v>31</v>
+        <v>35</v>
       </c>
       <c r="V2" s="4" t="s">
-        <v>28</v>
+        <v>32</v>
       </c>
       <c r="W2" s="4" t="s">
-        <v>29</v>
+        <v>33</v>
       </c>
       <c r="X2" s="4" t="s">
-        <v>30</v>
+        <v>34</v>
       </c>
       <c r="Y2" s="4" t="s">
-        <v>31</v>
+        <v>35</v>
       </c>
       <c r="Z2" s="4" t="s">
-        <v>28</v>
+        <v>32</v>
       </c>
       <c r="AA2" s="4" t="s">
-        <v>29</v>
+        <v>33</v>
       </c>
       <c r="AB2" s="4" t="s">
-        <v>30</v>
+        <v>34</v>
       </c>
       <c r="AC2" s="4" t="s">
-        <v>31</v>
+        <v>35</v>
       </c>
       <c r="AD2" s="4" t="s">
-        <v>28</v>
+        <v>32</v>
       </c>
       <c r="AE2" s="4" t="s">
-        <v>29</v>
+        <v>33</v>
       </c>
       <c r="AF2" s="4" t="s">
-        <v>30</v>
+        <v>34</v>
       </c>
       <c r="AG2" s="4" t="s">
-        <v>31</v>
+        <v>35</v>
       </c>
       <c r="AH2" s="4" t="s">
-        <v>28</v>
+        <v>32</v>
       </c>
       <c r="AI2" s="4" t="s">
-        <v>29</v>
+        <v>33</v>
       </c>
       <c r="AJ2" s="4" t="s">
-        <v>30</v>
+        <v>34</v>
       </c>
       <c r="AK2" s="4" t="s">
-        <v>31</v>
+        <v>35</v>
       </c>
       <c r="AL2" s="4" t="s">
-        <v>28</v>
+        <v>32</v>
       </c>
       <c r="AM2" s="4" t="s">
-        <v>29</v>
+        <v>33</v>
       </c>
       <c r="AN2" s="4" t="s">
-        <v>30</v>
+        <v>34</v>
       </c>
       <c r="AO2" s="4" t="s">
-        <v>31</v>
+        <v>35</v>
       </c>
       <c r="AP2" s="4" t="s">
-        <v>28</v>
+        <v>32</v>
       </c>
       <c r="AQ2" s="4" t="s">
-        <v>29</v>
+        <v>33</v>
       </c>
       <c r="AR2" s="4" t="s">
-        <v>30</v>
+        <v>34</v>
       </c>
       <c r="AS2" s="4" t="s">
-        <v>31</v>
+        <v>35</v>
       </c>
       <c r="AT2" s="4" t="s">
-        <v>28</v>
+        <v>32</v>
       </c>
       <c r="AU2" s="4" t="s">
-        <v>29</v>
+        <v>33</v>
       </c>
       <c r="AV2" s="4" t="s">
-        <v>30</v>
+        <v>34</v>
       </c>
       <c r="AW2" s="4" t="s">
-        <v>31</v>
+        <v>35</v>
       </c>
       <c r="AX2" s="4" t="s">
-        <v>28</v>
+        <v>32</v>
       </c>
       <c r="AY2" s="4" t="s">
-        <v>29</v>
+        <v>33</v>
       </c>
       <c r="AZ2" s="4" t="s">
-        <v>30</v>
+        <v>34</v>
       </c>
       <c r="BA2" s="4" t="s">
-        <v>31</v>
+        <v>35</v>
       </c>
       <c r="BB2" s="4" t="s">
-        <v>28</v>
+        <v>32</v>
       </c>
       <c r="BC2" s="4" t="s">
-        <v>29</v>
+        <v>33</v>
       </c>
       <c r="BD2" s="4" t="s">
-        <v>30</v>
+        <v>34</v>
       </c>
       <c r="BE2" s="4" t="s">
-        <v>31</v>
+        <v>35</v>
       </c>
       <c r="BF2" s="4" t="s">
-        <v>28</v>
+        <v>32</v>
       </c>
       <c r="BG2" s="4" t="s">
-        <v>29</v>
+        <v>33</v>
       </c>
       <c r="BH2" s="4" t="s">
-        <v>30</v>
+        <v>34</v>
       </c>
       <c r="BI2" s="4" t="s">
-        <v>31</v>
+        <v>35</v>
       </c>
       <c r="BJ2" s="4" t="s">
-        <v>28</v>
+        <v>32</v>
       </c>
       <c r="BK2" s="4" t="s">
-        <v>29</v>
+        <v>33</v>
       </c>
       <c r="BL2" s="4" t="s">
-        <v>30</v>
+        <v>34</v>
       </c>
       <c r="BM2" s="4" t="s">
-        <v>31</v>
+        <v>35</v>
       </c>
       <c r="BN2" s="4" t="s">
-        <v>28</v>
+        <v>32</v>
       </c>
       <c r="BO2" s="4" t="s">
-        <v>29</v>
+        <v>33</v>
       </c>
       <c r="BP2" s="4" t="s">
-        <v>30</v>
+        <v>34</v>
       </c>
       <c r="BQ2" s="4" t="s">
-        <v>31</v>
+        <v>35</v>
       </c>
       <c r="BR2" s="4" t="s">
-        <v>28</v>
+        <v>32</v>
       </c>
       <c r="BS2" s="4" t="s">
-        <v>29</v>
+        <v>33</v>
       </c>
       <c r="BT2" s="4" t="s">
-        <v>30</v>
+        <v>34</v>
       </c>
       <c r="BU2" s="4" t="s">
-        <v>31</v>
+        <v>35</v>
       </c>
       <c r="BV2" s="4" t="s">
-        <v>28</v>
+        <v>32</v>
       </c>
       <c r="BW2" s="4" t="s">
-        <v>29</v>
+        <v>33</v>
       </c>
       <c r="BX2" s="4" t="s">
-        <v>30</v>
+        <v>34</v>
       </c>
       <c r="BY2" s="4" t="s">
-        <v>31</v>
+        <v>35</v>
       </c>
       <c r="BZ2" s="4" t="s">
-        <v>28</v>
+        <v>32</v>
       </c>
       <c r="CA2" s="4" t="s">
-        <v>29</v>
+        <v>33</v>
       </c>
       <c r="CB2" s="4" t="s">
-        <v>30</v>
+        <v>34</v>
       </c>
       <c r="CC2" s="4" t="s">
-        <v>31</v>
+        <v>35</v>
+      </c>
+      <c r="CD2" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="CE2" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="CF2" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="CG2" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="CH2" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="CI2" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="CJ2" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="CK2" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="CL2" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="CM2" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="CN2" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="CO2" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="CP2" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="CQ2" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="CR2" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="CS2" s="4" t="s">
+        <v>35</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="5" t="s">
-        <v>32</v>
+        <v>36</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>33</v>
+        <v>37</v>
       </c>
       <c r="C3" s="5"/>
       <c r="D3" s="5"/>
@@ -783,7 +875,7 @@
       <c r="O3" s="7"/>
       <c r="P3" s="7"/>
       <c r="Q3" s="7" t="n">
-        <v>210</v>
+        <v>126</v>
       </c>
       <c r="R3" s="7" t="n">
         <v>179</v>
@@ -791,7 +883,7 @@
       <c r="S3" s="7"/>
       <c r="T3" s="7"/>
       <c r="U3" s="7" t="n">
-        <v>392</v>
+        <v>182</v>
       </c>
       <c r="V3" s="7" t="n">
         <v>251</v>
@@ -799,7 +891,7 @@
       <c r="W3" s="7"/>
       <c r="X3" s="7"/>
       <c r="Y3" s="7" t="n">
-        <v>623</v>
+        <v>231</v>
       </c>
       <c r="Z3" s="7" t="n">
         <v>394</v>
@@ -807,7 +899,7 @@
       <c r="AA3" s="7"/>
       <c r="AB3" s="7"/>
       <c r="AC3" s="7" t="n">
-        <v>889</v>
+        <v>266</v>
       </c>
       <c r="AD3" s="7" t="n">
         <v>451</v>
@@ -815,7 +907,7 @@
       <c r="AE3" s="7"/>
       <c r="AF3" s="7"/>
       <c r="AG3" s="7" t="n">
-        <v>1190</v>
+        <v>301</v>
       </c>
       <c r="AH3" s="7" t="n">
         <v>554</v>
@@ -823,7 +915,7 @@
       <c r="AI3" s="7"/>
       <c r="AJ3" s="7"/>
       <c r="AK3" s="7" t="n">
-        <v>1519</v>
+        <v>329</v>
       </c>
       <c r="AL3" s="7" t="n">
         <v>649</v>
@@ -831,7 +923,7 @@
       <c r="AM3" s="7"/>
       <c r="AN3" s="7"/>
       <c r="AO3" s="7" t="n">
-        <v>1876</v>
+        <v>357</v>
       </c>
       <c r="AP3" s="7" t="n">
         <v>738</v>
@@ -839,7 +931,7 @@
       <c r="AQ3" s="7"/>
       <c r="AR3" s="7"/>
       <c r="AS3" s="7" t="n">
-        <v>2261</v>
+        <v>385</v>
       </c>
       <c r="AT3" s="7" t="n">
         <v>830</v>
@@ -847,7 +939,7 @@
       <c r="AU3" s="7"/>
       <c r="AV3" s="7"/>
       <c r="AW3" s="7" t="n">
-        <v>2674</v>
+        <v>413</v>
       </c>
       <c r="AX3" s="7" t="n">
         <v>923</v>
@@ -855,7 +947,7 @@
       <c r="AY3" s="7"/>
       <c r="AZ3" s="7"/>
       <c r="BA3" s="7" t="n">
-        <v>3108</v>
+        <v>434</v>
       </c>
       <c r="BB3" s="7" t="n">
         <v>1025</v>
@@ -863,7 +955,7 @@
       <c r="BC3" s="7"/>
       <c r="BD3" s="7"/>
       <c r="BE3" s="7" t="n">
-        <v>3563</v>
+        <v>455</v>
       </c>
       <c r="BF3" s="7" t="n">
         <v>1122</v>
@@ -871,7 +963,7 @@
       <c r="BG3" s="7"/>
       <c r="BH3" s="7"/>
       <c r="BI3" s="7" t="n">
-        <v>4039</v>
+        <v>476</v>
       </c>
       <c r="BJ3" s="7" t="n">
         <v>1210</v>
@@ -879,7 +971,7 @@
       <c r="BK3" s="7"/>
       <c r="BL3" s="7"/>
       <c r="BM3" s="7" t="n">
-        <v>4536</v>
+        <v>497</v>
       </c>
       <c r="BN3" s="7" t="n">
         <v>1297</v>
@@ -887,7 +979,7 @@
       <c r="BO3" s="7"/>
       <c r="BP3" s="7"/>
       <c r="BQ3" s="7" t="n">
-        <v>5054</v>
+        <v>518</v>
       </c>
       <c r="BR3" s="7" t="n">
         <v>1384</v>
@@ -895,7 +987,7 @@
       <c r="BS3" s="7"/>
       <c r="BT3" s="7"/>
       <c r="BU3" s="7" t="n">
-        <v>5593</v>
+        <v>539</v>
       </c>
       <c r="BV3" s="7" t="n">
         <v>1461</v>
@@ -903,15 +995,67 @@
       <c r="BW3" s="7"/>
       <c r="BX3" s="7"/>
       <c r="BY3" s="7" t="n">
-        <v>6160</v>
+        <v>567</v>
       </c>
       <c r="BZ3" s="7" t="n">
         <v>1538</v>
       </c>
-      <c r="CA3" s="7"/>
-      <c r="CB3" s="7"/>
+      <c r="CA3" s="7" t="n">
+        <v>1</v>
+      </c>
+      <c r="CB3" s="7" t="n">
+        <v>50</v>
+      </c>
       <c r="CC3" s="7" t="n">
-        <v>6769</v>
+        <v>609</v>
+      </c>
+      <c r="CD3" s="7" t="n">
+        <v>1560</v>
+      </c>
+      <c r="CE3" s="7" t="n">
+        <v>2</v>
+      </c>
+      <c r="CF3" s="7" t="n">
+        <v>112</v>
+      </c>
+      <c r="CG3" s="7" t="n">
+        <v>621</v>
+      </c>
+      <c r="CH3" s="7" t="n">
+        <v>1610</v>
+      </c>
+      <c r="CI3" s="7" t="n">
+        <v>4</v>
+      </c>
+      <c r="CJ3" s="7" t="n">
+        <v>260</v>
+      </c>
+      <c r="CK3" s="7" t="n">
+        <v>645</v>
+      </c>
+      <c r="CL3" s="7" t="n">
+        <v>1665</v>
+      </c>
+      <c r="CM3" s="7" t="n">
+        <v>2</v>
+      </c>
+      <c r="CN3" s="7" t="n">
+        <v>152</v>
+      </c>
+      <c r="CO3" s="7" t="n">
+        <v>670</v>
+      </c>
+      <c r="CP3" s="7" t="n">
+        <v>1710</v>
+      </c>
+      <c r="CQ3" s="7" t="n">
+        <v>5</v>
+      </c>
+      <c r="CR3" s="7" t="n">
+        <v>250</v>
+      </c>
+      <c r="CS3" s="7" t="n">
+        <v>690</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -936,6 +1080,10 @@
       <c r="BR8" s="8"/>
       <c r="BV8" s="8"/>
       <c r="BZ8" s="8"/>
+      <c r="CD8" s="8"/>
+      <c r="CH8" s="8"/>
+      <c r="CL8" s="8"/>
+      <c r="CP8" s="8"/>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="F9" s="1"/>
@@ -946,7 +1094,7 @@
       <c r="C10" s="1"/>
       <c r="D10" s="1"/>
       <c r="E10" s="1"/>
-      <c r="F10" s="0"/>
+      <c r="F10" s="1"/>
       <c r="G10" s="1"/>
       <c r="H10" s="1"/>
       <c r="I10" s="1"/>
@@ -1022,9 +1170,25 @@
       <c r="CA10" s="1"/>
       <c r="CB10" s="1"/>
       <c r="CC10" s="1"/>
+      <c r="CD10" s="1"/>
+      <c r="CE10" s="1"/>
+      <c r="CF10" s="1"/>
+      <c r="CG10" s="1"/>
+      <c r="CH10" s="1"/>
+      <c r="CI10" s="1"/>
+      <c r="CJ10" s="1"/>
+      <c r="CK10" s="1"/>
+      <c r="CL10" s="1"/>
+      <c r="CM10" s="1"/>
+      <c r="CN10" s="1"/>
+      <c r="CO10" s="1"/>
+      <c r="CP10" s="1"/>
+      <c r="CQ10" s="1"/>
+      <c r="CR10" s="1"/>
+      <c r="CS10" s="1"/>
     </row>
   </sheetData>
-  <mergeCells count="19">
+  <mergeCells count="23">
     <mergeCell ref="A1:F1"/>
     <mergeCell ref="J1:M1"/>
     <mergeCell ref="N1:Q1"/>
@@ -1044,6 +1208,10 @@
     <mergeCell ref="BR1:BU1"/>
     <mergeCell ref="BV1:BY1"/>
     <mergeCell ref="BZ1:CC1"/>
+    <mergeCell ref="CD1:CG1"/>
+    <mergeCell ref="CH1:CK1"/>
+    <mergeCell ref="CL1:CO1"/>
+    <mergeCell ref="CP1:CS1"/>
   </mergeCells>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>

</xml_diff>

<commit_message>
chicken import with breed type and farm
</commit_message>
<xml_diff>
--- a/bovan_brown_max.xlsx
+++ b/bovan_brown_max.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="122" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="312" uniqueCount="76">
   <si>
     <t xml:space="preserve">Weeks</t>
   </si>
@@ -89,6 +89,120 @@
   </si>
   <si>
     <t xml:space="preserve">Week 22</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Week 23</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Week 24</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Week 25</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Week 26</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Week 27</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Week 28</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Week 29</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Week 30</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Week 31</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Week 32</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Week 33</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Week 34</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Week 35</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Week 36</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Week 37</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Week 38</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Week 39</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Week 40</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Week 41</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Week 42</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Week 43</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Week 44</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Week 45</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Week 46</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Week 47</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Week 48</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Week 49</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Week 50</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Week 51</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Week 52</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Week 53</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Week 54</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Week 55</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Week 56</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Week 57</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Week 58</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Week 59</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Week 60</t>
   </si>
   <si>
     <t xml:space="preserve">ID</t>
@@ -343,10 +457,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:CS10"/>
+  <dimension ref="A1:IS10"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="BR1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="CR3" activeCellId="0" sqref="CR3"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="GV1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="HU11" activeCellId="0" sqref="HU11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -403,6 +517,82 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="93" min="91" style="1" width="7.18"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="94" min="94" style="1" width="7.3"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="97" min="95" style="1" width="7.18"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="98" min="98" style="1" width="7.3"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="101" min="99" style="1" width="7.18"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="102" min="102" style="1" width="7.3"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="105" min="103" style="1" width="7.18"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="106" min="106" style="1" width="7.3"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="109" min="107" style="1" width="7.18"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="110" min="110" style="1" width="7.3"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="113" min="111" style="1" width="7.18"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="114" min="114" style="1" width="7.3"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="117" min="115" style="1" width="7.18"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="118" min="118" style="1" width="7.3"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="121" min="119" style="1" width="7.18"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="122" min="122" style="1" width="7.3"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="125" min="123" style="1" width="7.18"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="126" min="126" style="1" width="7.3"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="129" min="127" style="1" width="7.18"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="130" min="130" style="1" width="7.3"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="133" min="131" style="1" width="7.18"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="134" min="134" style="1" width="7.3"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="137" min="135" style="1" width="7.18"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="138" min="138" style="1" width="7.3"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="141" min="139" style="1" width="7.18"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="142" min="142" style="1" width="7.3"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="145" min="143" style="1" width="7.18"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="146" min="146" style="1" width="7.3"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="149" min="147" style="1" width="7.18"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="150" min="150" style="1" width="7.3"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="153" min="151" style="1" width="7.18"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="154" min="154" style="1" width="7.3"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="157" min="155" style="1" width="7.18"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="158" min="158" style="1" width="7.3"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="161" min="159" style="1" width="7.18"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="162" min="162" style="1" width="7.3"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="165" min="163" style="1" width="7.18"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="166" min="166" style="1" width="7.3"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="169" min="167" style="1" width="7.18"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="170" min="170" style="1" width="7.3"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="173" min="171" style="1" width="7.18"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="174" min="174" style="1" width="7.3"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="177" min="175" style="1" width="7.18"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="178" min="178" style="1" width="7.3"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="181" min="179" style="1" width="7.18"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="182" min="182" style="1" width="7.3"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="185" min="183" style="1" width="7.18"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="186" min="186" style="1" width="7.3"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="189" min="187" style="1" width="7.18"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="190" min="190" style="1" width="7.3"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="193" min="191" style="1" width="7.18"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="194" min="194" style="1" width="7.3"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="197" min="195" style="1" width="7.18"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="198" min="198" style="1" width="7.3"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="201" min="199" style="1" width="7.18"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="202" min="202" style="1" width="7.3"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="205" min="203" style="1" width="7.18"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="206" min="206" style="1" width="7.3"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="209" min="207" style="1" width="7.18"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="210" min="210" style="1" width="7.3"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="213" min="211" style="1" width="7.18"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="214" min="214" style="1" width="7.3"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="217" min="215" style="1" width="7.18"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="218" min="218" style="1" width="7.3"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="221" min="219" style="1" width="7.18"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="222" min="222" style="1" width="7.3"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="225" min="223" style="1" width="7.18"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="226" min="226" style="1" width="7.3"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="229" min="227" style="1" width="7.18"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="230" min="230" style="1" width="7.3"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="233" min="231" style="1" width="7.18"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="234" min="234" style="1" width="7.3"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="237" min="235" style="1" width="7.18"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="238" min="238" style="1" width="7.3"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="241" min="239" style="1" width="7.18"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="242" min="242" style="1" width="7.3"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="245" min="243" style="1" width="7.18"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="246" min="246" style="1" width="7.3"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="249" min="247" style="1" width="7.18"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="29.85" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -549,306 +739,990 @@
       <c r="CQ1" s="3"/>
       <c r="CR1" s="3"/>
       <c r="CS1" s="3"/>
+      <c r="CT1" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="CU1" s="3"/>
+      <c r="CV1" s="3"/>
+      <c r="CW1" s="3"/>
+      <c r="CX1" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="CY1" s="3"/>
+      <c r="CZ1" s="3"/>
+      <c r="DA1" s="3"/>
+      <c r="DB1" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="DC1" s="3"/>
+      <c r="DD1" s="3"/>
+      <c r="DE1" s="3"/>
+      <c r="DF1" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="DG1" s="3"/>
+      <c r="DH1" s="3"/>
+      <c r="DI1" s="3"/>
+      <c r="DJ1" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="DK1" s="3"/>
+      <c r="DL1" s="3"/>
+      <c r="DM1" s="3"/>
+      <c r="DN1" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="DO1" s="3"/>
+      <c r="DP1" s="3"/>
+      <c r="DQ1" s="3"/>
+      <c r="DR1" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="DS1" s="3"/>
+      <c r="DT1" s="3"/>
+      <c r="DU1" s="3"/>
+      <c r="DV1" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="DW1" s="3"/>
+      <c r="DX1" s="3"/>
+      <c r="DY1" s="3"/>
+      <c r="DZ1" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="EA1" s="3"/>
+      <c r="EB1" s="3"/>
+      <c r="EC1" s="3"/>
+      <c r="ED1" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="EE1" s="3"/>
+      <c r="EF1" s="3"/>
+      <c r="EG1" s="3"/>
+      <c r="EH1" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="EI1" s="3"/>
+      <c r="EJ1" s="3"/>
+      <c r="EK1" s="3"/>
+      <c r="EL1" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="EM1" s="3"/>
+      <c r="EN1" s="3"/>
+      <c r="EO1" s="3"/>
+      <c r="EP1" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="EQ1" s="3"/>
+      <c r="ER1" s="3"/>
+      <c r="ES1" s="3"/>
+      <c r="ET1" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="EU1" s="3"/>
+      <c r="EV1" s="3"/>
+      <c r="EW1" s="3"/>
+      <c r="EX1" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="EY1" s="3"/>
+      <c r="EZ1" s="3"/>
+      <c r="FA1" s="3"/>
+      <c r="FB1" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="FC1" s="3"/>
+      <c r="FD1" s="3"/>
+      <c r="FE1" s="3"/>
+      <c r="FF1" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="FG1" s="3"/>
+      <c r="FH1" s="3"/>
+      <c r="FI1" s="3"/>
+      <c r="FJ1" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="FK1" s="3"/>
+      <c r="FL1" s="3"/>
+      <c r="FM1" s="3"/>
+      <c r="FN1" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="FO1" s="3"/>
+      <c r="FP1" s="3"/>
+      <c r="FQ1" s="3"/>
+      <c r="FR1" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="FS1" s="3"/>
+      <c r="FT1" s="3"/>
+      <c r="FU1" s="3"/>
+      <c r="FV1" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="FW1" s="3"/>
+      <c r="FX1" s="3"/>
+      <c r="FY1" s="3"/>
+      <c r="FZ1" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="GA1" s="3"/>
+      <c r="GB1" s="3"/>
+      <c r="GC1" s="3"/>
+      <c r="GD1" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="GE1" s="3"/>
+      <c r="GF1" s="3"/>
+      <c r="GG1" s="3"/>
+      <c r="GH1" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="GI1" s="3"/>
+      <c r="GJ1" s="3"/>
+      <c r="GK1" s="3"/>
+      <c r="GL1" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="GM1" s="3"/>
+      <c r="GN1" s="3"/>
+      <c r="GO1" s="3"/>
+      <c r="GP1" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="GQ1" s="3"/>
+      <c r="GR1" s="3"/>
+      <c r="GS1" s="3"/>
+      <c r="GT1" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="GU1" s="3"/>
+      <c r="GV1" s="3"/>
+      <c r="GW1" s="3"/>
+      <c r="GX1" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="GY1" s="3"/>
+      <c r="GZ1" s="3"/>
+      <c r="HA1" s="3"/>
+      <c r="HB1" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="HC1" s="3"/>
+      <c r="HD1" s="3"/>
+      <c r="HE1" s="3"/>
+      <c r="HF1" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="HG1" s="3"/>
+      <c r="HH1" s="3"/>
+      <c r="HI1" s="3"/>
+      <c r="HJ1" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="HK1" s="3"/>
+      <c r="HL1" s="3"/>
+      <c r="HM1" s="3"/>
+      <c r="HN1" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="HO1" s="3"/>
+      <c r="HP1" s="3"/>
+      <c r="HQ1" s="3"/>
+      <c r="HR1" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="HS1" s="3"/>
+      <c r="HT1" s="3"/>
+      <c r="HU1" s="3"/>
+      <c r="HV1" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="HW1" s="3"/>
+      <c r="HX1" s="3"/>
+      <c r="HY1" s="3"/>
+      <c r="HZ1" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="IA1" s="3"/>
+      <c r="IB1" s="3"/>
+      <c r="IC1" s="3"/>
+      <c r="ID1" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="IE1" s="3"/>
+      <c r="IF1" s="3"/>
+      <c r="IG1" s="3"/>
+      <c r="IH1" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="II1" s="3"/>
+      <c r="IJ1" s="3"/>
+      <c r="IK1" s="3"/>
+      <c r="IL1" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="IM1" s="3"/>
+      <c r="IN1" s="3"/>
+      <c r="IO1" s="3"/>
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="4" t="s">
-        <v>23</v>
+        <v>61</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>24</v>
+        <v>62</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>25</v>
+        <v>63</v>
       </c>
       <c r="D2" s="4" t="s">
-        <v>26</v>
+        <v>64</v>
       </c>
       <c r="E2" s="4" t="s">
-        <v>27</v>
+        <v>65</v>
       </c>
       <c r="F2" s="4" t="s">
-        <v>28</v>
+        <v>66</v>
       </c>
       <c r="G2" s="4" t="s">
-        <v>29</v>
+        <v>67</v>
       </c>
       <c r="H2" s="4" t="s">
-        <v>30</v>
+        <v>68</v>
       </c>
       <c r="I2" s="4" t="s">
-        <v>31</v>
+        <v>69</v>
       </c>
       <c r="J2" s="4" t="s">
-        <v>32</v>
+        <v>70</v>
       </c>
       <c r="K2" s="4" t="s">
-        <v>33</v>
+        <v>71</v>
       </c>
       <c r="L2" s="4" t="s">
-        <v>34</v>
+        <v>72</v>
       </c>
       <c r="M2" s="4" t="s">
-        <v>35</v>
+        <v>73</v>
       </c>
       <c r="N2" s="4" t="s">
-        <v>32</v>
+        <v>70</v>
       </c>
       <c r="O2" s="4" t="s">
-        <v>33</v>
+        <v>71</v>
       </c>
       <c r="P2" s="4" t="s">
-        <v>34</v>
+        <v>72</v>
       </c>
       <c r="Q2" s="4" t="s">
-        <v>35</v>
+        <v>73</v>
       </c>
       <c r="R2" s="4" t="s">
-        <v>32</v>
+        <v>70</v>
       </c>
       <c r="S2" s="4" t="s">
-        <v>33</v>
+        <v>71</v>
       </c>
       <c r="T2" s="4" t="s">
-        <v>34</v>
+        <v>72</v>
       </c>
       <c r="U2" s="4" t="s">
-        <v>35</v>
+        <v>73</v>
       </c>
       <c r="V2" s="4" t="s">
-        <v>32</v>
+        <v>70</v>
       </c>
       <c r="W2" s="4" t="s">
-        <v>33</v>
+        <v>71</v>
       </c>
       <c r="X2" s="4" t="s">
-        <v>34</v>
+        <v>72</v>
       </c>
       <c r="Y2" s="4" t="s">
-        <v>35</v>
+        <v>73</v>
       </c>
       <c r="Z2" s="4" t="s">
-        <v>32</v>
+        <v>70</v>
       </c>
       <c r="AA2" s="4" t="s">
-        <v>33</v>
+        <v>71</v>
       </c>
       <c r="AB2" s="4" t="s">
-        <v>34</v>
+        <v>72</v>
       </c>
       <c r="AC2" s="4" t="s">
-        <v>35</v>
+        <v>73</v>
       </c>
       <c r="AD2" s="4" t="s">
-        <v>32</v>
+        <v>70</v>
       </c>
       <c r="AE2" s="4" t="s">
-        <v>33</v>
+        <v>71</v>
       </c>
       <c r="AF2" s="4" t="s">
-        <v>34</v>
+        <v>72</v>
       </c>
       <c r="AG2" s="4" t="s">
-        <v>35</v>
+        <v>73</v>
       </c>
       <c r="AH2" s="4" t="s">
-        <v>32</v>
+        <v>70</v>
       </c>
       <c r="AI2" s="4" t="s">
-        <v>33</v>
+        <v>71</v>
       </c>
       <c r="AJ2" s="4" t="s">
-        <v>34</v>
+        <v>72</v>
       </c>
       <c r="AK2" s="4" t="s">
-        <v>35</v>
+        <v>73</v>
       </c>
       <c r="AL2" s="4" t="s">
-        <v>32</v>
+        <v>70</v>
       </c>
       <c r="AM2" s="4" t="s">
-        <v>33</v>
+        <v>71</v>
       </c>
       <c r="AN2" s="4" t="s">
-        <v>34</v>
+        <v>72</v>
       </c>
       <c r="AO2" s="4" t="s">
-        <v>35</v>
+        <v>73</v>
       </c>
       <c r="AP2" s="4" t="s">
-        <v>32</v>
+        <v>70</v>
       </c>
       <c r="AQ2" s="4" t="s">
-        <v>33</v>
+        <v>71</v>
       </c>
       <c r="AR2" s="4" t="s">
-        <v>34</v>
+        <v>72</v>
       </c>
       <c r="AS2" s="4" t="s">
-        <v>35</v>
+        <v>73</v>
       </c>
       <c r="AT2" s="4" t="s">
-        <v>32</v>
+        <v>70</v>
       </c>
       <c r="AU2" s="4" t="s">
-        <v>33</v>
+        <v>71</v>
       </c>
       <c r="AV2" s="4" t="s">
-        <v>34</v>
+        <v>72</v>
       </c>
       <c r="AW2" s="4" t="s">
-        <v>35</v>
+        <v>73</v>
       </c>
       <c r="AX2" s="4" t="s">
-        <v>32</v>
+        <v>70</v>
       </c>
       <c r="AY2" s="4" t="s">
-        <v>33</v>
+        <v>71</v>
       </c>
       <c r="AZ2" s="4" t="s">
-        <v>34</v>
+        <v>72</v>
       </c>
       <c r="BA2" s="4" t="s">
-        <v>35</v>
+        <v>73</v>
       </c>
       <c r="BB2" s="4" t="s">
-        <v>32</v>
+        <v>70</v>
       </c>
       <c r="BC2" s="4" t="s">
-        <v>33</v>
+        <v>71</v>
       </c>
       <c r="BD2" s="4" t="s">
-        <v>34</v>
+        <v>72</v>
       </c>
       <c r="BE2" s="4" t="s">
-        <v>35</v>
+        <v>73</v>
       </c>
       <c r="BF2" s="4" t="s">
-        <v>32</v>
+        <v>70</v>
       </c>
       <c r="BG2" s="4" t="s">
-        <v>33</v>
+        <v>71</v>
       </c>
       <c r="BH2" s="4" t="s">
-        <v>34</v>
+        <v>72</v>
       </c>
       <c r="BI2" s="4" t="s">
-        <v>35</v>
+        <v>73</v>
       </c>
       <c r="BJ2" s="4" t="s">
-        <v>32</v>
+        <v>70</v>
       </c>
       <c r="BK2" s="4" t="s">
-        <v>33</v>
+        <v>71</v>
       </c>
       <c r="BL2" s="4" t="s">
-        <v>34</v>
+        <v>72</v>
       </c>
       <c r="BM2" s="4" t="s">
-        <v>35</v>
+        <v>73</v>
       </c>
       <c r="BN2" s="4" t="s">
-        <v>32</v>
+        <v>70</v>
       </c>
       <c r="BO2" s="4" t="s">
-        <v>33</v>
+        <v>71</v>
       </c>
       <c r="BP2" s="4" t="s">
-        <v>34</v>
+        <v>72</v>
       </c>
       <c r="BQ2" s="4" t="s">
-        <v>35</v>
+        <v>73</v>
       </c>
       <c r="BR2" s="4" t="s">
-        <v>32</v>
+        <v>70</v>
       </c>
       <c r="BS2" s="4" t="s">
-        <v>33</v>
+        <v>71</v>
       </c>
       <c r="BT2" s="4" t="s">
-        <v>34</v>
+        <v>72</v>
       </c>
       <c r="BU2" s="4" t="s">
-        <v>35</v>
+        <v>73</v>
       </c>
       <c r="BV2" s="4" t="s">
-        <v>32</v>
+        <v>70</v>
       </c>
       <c r="BW2" s="4" t="s">
-        <v>33</v>
+        <v>71</v>
       </c>
       <c r="BX2" s="4" t="s">
-        <v>34</v>
+        <v>72</v>
       </c>
       <c r="BY2" s="4" t="s">
-        <v>35</v>
+        <v>73</v>
       </c>
       <c r="BZ2" s="4" t="s">
-        <v>32</v>
+        <v>70</v>
       </c>
       <c r="CA2" s="4" t="s">
-        <v>33</v>
+        <v>71</v>
       </c>
       <c r="CB2" s="4" t="s">
-        <v>34</v>
+        <v>72</v>
       </c>
       <c r="CC2" s="4" t="s">
-        <v>35</v>
+        <v>73</v>
       </c>
       <c r="CD2" s="4" t="s">
-        <v>32</v>
+        <v>70</v>
       </c>
       <c r="CE2" s="4" t="s">
-        <v>33</v>
+        <v>71</v>
       </c>
       <c r="CF2" s="4" t="s">
-        <v>34</v>
+        <v>72</v>
       </c>
       <c r="CG2" s="4" t="s">
-        <v>35</v>
+        <v>73</v>
       </c>
       <c r="CH2" s="4" t="s">
-        <v>32</v>
+        <v>70</v>
       </c>
       <c r="CI2" s="4" t="s">
-        <v>33</v>
+        <v>71</v>
       </c>
       <c r="CJ2" s="4" t="s">
-        <v>34</v>
+        <v>72</v>
       </c>
       <c r="CK2" s="4" t="s">
-        <v>35</v>
+        <v>73</v>
       </c>
       <c r="CL2" s="4" t="s">
-        <v>32</v>
+        <v>70</v>
       </c>
       <c r="CM2" s="4" t="s">
-        <v>33</v>
+        <v>71</v>
       </c>
       <c r="CN2" s="4" t="s">
-        <v>34</v>
+        <v>72</v>
       </c>
       <c r="CO2" s="4" t="s">
-        <v>35</v>
+        <v>73</v>
       </c>
       <c r="CP2" s="4" t="s">
-        <v>32</v>
+        <v>70</v>
       </c>
       <c r="CQ2" s="4" t="s">
-        <v>33</v>
+        <v>71</v>
       </c>
       <c r="CR2" s="4" t="s">
-        <v>34</v>
+        <v>72</v>
       </c>
       <c r="CS2" s="4" t="s">
-        <v>35</v>
+        <v>73</v>
+      </c>
+      <c r="CT2" s="4" t="s">
+        <v>70</v>
+      </c>
+      <c r="CU2" s="4" t="s">
+        <v>71</v>
+      </c>
+      <c r="CV2" s="4" t="s">
+        <v>72</v>
+      </c>
+      <c r="CW2" s="4" t="s">
+        <v>73</v>
+      </c>
+      <c r="CX2" s="4" t="s">
+        <v>70</v>
+      </c>
+      <c r="CY2" s="4" t="s">
+        <v>71</v>
+      </c>
+      <c r="CZ2" s="4" t="s">
+        <v>72</v>
+      </c>
+      <c r="DA2" s="4" t="s">
+        <v>73</v>
+      </c>
+      <c r="DB2" s="4" t="s">
+        <v>70</v>
+      </c>
+      <c r="DC2" s="4" t="s">
+        <v>71</v>
+      </c>
+      <c r="DD2" s="4" t="s">
+        <v>72</v>
+      </c>
+      <c r="DE2" s="4" t="s">
+        <v>73</v>
+      </c>
+      <c r="DF2" s="4" t="s">
+        <v>70</v>
+      </c>
+      <c r="DG2" s="4" t="s">
+        <v>71</v>
+      </c>
+      <c r="DH2" s="4" t="s">
+        <v>72</v>
+      </c>
+      <c r="DI2" s="4" t="s">
+        <v>73</v>
+      </c>
+      <c r="DJ2" s="4" t="s">
+        <v>70</v>
+      </c>
+      <c r="DK2" s="4" t="s">
+        <v>71</v>
+      </c>
+      <c r="DL2" s="4" t="s">
+        <v>72</v>
+      </c>
+      <c r="DM2" s="4" t="s">
+        <v>73</v>
+      </c>
+      <c r="DN2" s="4" t="s">
+        <v>70</v>
+      </c>
+      <c r="DO2" s="4" t="s">
+        <v>71</v>
+      </c>
+      <c r="DP2" s="4" t="s">
+        <v>72</v>
+      </c>
+      <c r="DQ2" s="4" t="s">
+        <v>73</v>
+      </c>
+      <c r="DR2" s="4" t="s">
+        <v>70</v>
+      </c>
+      <c r="DS2" s="4" t="s">
+        <v>71</v>
+      </c>
+      <c r="DT2" s="4" t="s">
+        <v>72</v>
+      </c>
+      <c r="DU2" s="4" t="s">
+        <v>73</v>
+      </c>
+      <c r="DV2" s="4" t="s">
+        <v>70</v>
+      </c>
+      <c r="DW2" s="4" t="s">
+        <v>71</v>
+      </c>
+      <c r="DX2" s="4" t="s">
+        <v>72</v>
+      </c>
+      <c r="DY2" s="4" t="s">
+        <v>73</v>
+      </c>
+      <c r="DZ2" s="4" t="s">
+        <v>70</v>
+      </c>
+      <c r="EA2" s="4" t="s">
+        <v>71</v>
+      </c>
+      <c r="EB2" s="4" t="s">
+        <v>72</v>
+      </c>
+      <c r="EC2" s="4" t="s">
+        <v>73</v>
+      </c>
+      <c r="ED2" s="4" t="s">
+        <v>70</v>
+      </c>
+      <c r="EE2" s="4" t="s">
+        <v>71</v>
+      </c>
+      <c r="EF2" s="4" t="s">
+        <v>72</v>
+      </c>
+      <c r="EG2" s="4" t="s">
+        <v>73</v>
+      </c>
+      <c r="EH2" s="4" t="s">
+        <v>70</v>
+      </c>
+      <c r="EI2" s="4" t="s">
+        <v>71</v>
+      </c>
+      <c r="EJ2" s="4" t="s">
+        <v>72</v>
+      </c>
+      <c r="EK2" s="4" t="s">
+        <v>73</v>
+      </c>
+      <c r="EL2" s="4" t="s">
+        <v>70</v>
+      </c>
+      <c r="EM2" s="4" t="s">
+        <v>71</v>
+      </c>
+      <c r="EN2" s="4" t="s">
+        <v>72</v>
+      </c>
+      <c r="EO2" s="4" t="s">
+        <v>73</v>
+      </c>
+      <c r="EP2" s="4" t="s">
+        <v>70</v>
+      </c>
+      <c r="EQ2" s="4" t="s">
+        <v>71</v>
+      </c>
+      <c r="ER2" s="4" t="s">
+        <v>72</v>
+      </c>
+      <c r="ES2" s="4" t="s">
+        <v>73</v>
+      </c>
+      <c r="ET2" s="4" t="s">
+        <v>70</v>
+      </c>
+      <c r="EU2" s="4" t="s">
+        <v>71</v>
+      </c>
+      <c r="EV2" s="4" t="s">
+        <v>72</v>
+      </c>
+      <c r="EW2" s="4" t="s">
+        <v>73</v>
+      </c>
+      <c r="EX2" s="4" t="s">
+        <v>70</v>
+      </c>
+      <c r="EY2" s="4" t="s">
+        <v>71</v>
+      </c>
+      <c r="EZ2" s="4" t="s">
+        <v>72</v>
+      </c>
+      <c r="FA2" s="4" t="s">
+        <v>73</v>
+      </c>
+      <c r="FB2" s="4" t="s">
+        <v>70</v>
+      </c>
+      <c r="FC2" s="4" t="s">
+        <v>71</v>
+      </c>
+      <c r="FD2" s="4" t="s">
+        <v>72</v>
+      </c>
+      <c r="FE2" s="4" t="s">
+        <v>73</v>
+      </c>
+      <c r="FF2" s="4" t="s">
+        <v>70</v>
+      </c>
+      <c r="FG2" s="4" t="s">
+        <v>71</v>
+      </c>
+      <c r="FH2" s="4" t="s">
+        <v>72</v>
+      </c>
+      <c r="FI2" s="4" t="s">
+        <v>73</v>
+      </c>
+      <c r="FJ2" s="4" t="s">
+        <v>70</v>
+      </c>
+      <c r="FK2" s="4" t="s">
+        <v>71</v>
+      </c>
+      <c r="FL2" s="4" t="s">
+        <v>72</v>
+      </c>
+      <c r="FM2" s="4" t="s">
+        <v>73</v>
+      </c>
+      <c r="FN2" s="4" t="s">
+        <v>70</v>
+      </c>
+      <c r="FO2" s="4" t="s">
+        <v>71</v>
+      </c>
+      <c r="FP2" s="4" t="s">
+        <v>72</v>
+      </c>
+      <c r="FQ2" s="4" t="s">
+        <v>73</v>
+      </c>
+      <c r="FR2" s="4" t="s">
+        <v>70</v>
+      </c>
+      <c r="FS2" s="4" t="s">
+        <v>71</v>
+      </c>
+      <c r="FT2" s="4" t="s">
+        <v>72</v>
+      </c>
+      <c r="FU2" s="4" t="s">
+        <v>73</v>
+      </c>
+      <c r="FV2" s="4" t="s">
+        <v>70</v>
+      </c>
+      <c r="FW2" s="4" t="s">
+        <v>71</v>
+      </c>
+      <c r="FX2" s="4" t="s">
+        <v>72</v>
+      </c>
+      <c r="FY2" s="4" t="s">
+        <v>73</v>
+      </c>
+      <c r="FZ2" s="4" t="s">
+        <v>70</v>
+      </c>
+      <c r="GA2" s="4" t="s">
+        <v>71</v>
+      </c>
+      <c r="GB2" s="4" t="s">
+        <v>72</v>
+      </c>
+      <c r="GC2" s="4" t="s">
+        <v>73</v>
+      </c>
+      <c r="GD2" s="4" t="s">
+        <v>70</v>
+      </c>
+      <c r="GE2" s="4" t="s">
+        <v>71</v>
+      </c>
+      <c r="GF2" s="4" t="s">
+        <v>72</v>
+      </c>
+      <c r="GG2" s="4" t="s">
+        <v>73</v>
+      </c>
+      <c r="GH2" s="4" t="s">
+        <v>70</v>
+      </c>
+      <c r="GI2" s="4" t="s">
+        <v>71</v>
+      </c>
+      <c r="GJ2" s="4" t="s">
+        <v>72</v>
+      </c>
+      <c r="GK2" s="4" t="s">
+        <v>73</v>
+      </c>
+      <c r="GL2" s="4" t="s">
+        <v>70</v>
+      </c>
+      <c r="GM2" s="4" t="s">
+        <v>71</v>
+      </c>
+      <c r="GN2" s="4" t="s">
+        <v>72</v>
+      </c>
+      <c r="GO2" s="4" t="s">
+        <v>73</v>
+      </c>
+      <c r="GP2" s="4" t="s">
+        <v>70</v>
+      </c>
+      <c r="GQ2" s="4" t="s">
+        <v>71</v>
+      </c>
+      <c r="GR2" s="4" t="s">
+        <v>72</v>
+      </c>
+      <c r="GS2" s="4" t="s">
+        <v>73</v>
+      </c>
+      <c r="GT2" s="4" t="s">
+        <v>70</v>
+      </c>
+      <c r="GU2" s="4" t="s">
+        <v>71</v>
+      </c>
+      <c r="GV2" s="4" t="s">
+        <v>72</v>
+      </c>
+      <c r="GW2" s="4" t="s">
+        <v>73</v>
+      </c>
+      <c r="GX2" s="4" t="s">
+        <v>70</v>
+      </c>
+      <c r="GY2" s="4" t="s">
+        <v>71</v>
+      </c>
+      <c r="GZ2" s="4" t="s">
+        <v>72</v>
+      </c>
+      <c r="HA2" s="4" t="s">
+        <v>73</v>
+      </c>
+      <c r="HB2" s="4" t="s">
+        <v>70</v>
+      </c>
+      <c r="HC2" s="4" t="s">
+        <v>71</v>
+      </c>
+      <c r="HD2" s="4" t="s">
+        <v>72</v>
+      </c>
+      <c r="HE2" s="4" t="s">
+        <v>73</v>
+      </c>
+      <c r="HF2" s="4" t="s">
+        <v>70</v>
+      </c>
+      <c r="HG2" s="4" t="s">
+        <v>71</v>
+      </c>
+      <c r="HH2" s="4" t="s">
+        <v>72</v>
+      </c>
+      <c r="HI2" s="4" t="s">
+        <v>73</v>
+      </c>
+      <c r="HJ2" s="4" t="s">
+        <v>70</v>
+      </c>
+      <c r="HK2" s="4" t="s">
+        <v>71</v>
+      </c>
+      <c r="HL2" s="4" t="s">
+        <v>72</v>
+      </c>
+      <c r="HM2" s="4" t="s">
+        <v>73</v>
+      </c>
+      <c r="HN2" s="4" t="s">
+        <v>70</v>
+      </c>
+      <c r="HO2" s="4" t="s">
+        <v>71</v>
+      </c>
+      <c r="HP2" s="4" t="s">
+        <v>72</v>
+      </c>
+      <c r="HQ2" s="4" t="s">
+        <v>73</v>
+      </c>
+      <c r="HR2" s="4" t="s">
+        <v>70</v>
+      </c>
+      <c r="HS2" s="4" t="s">
+        <v>71</v>
+      </c>
+      <c r="HT2" s="4" t="s">
+        <v>72</v>
+      </c>
+      <c r="HU2" s="4" t="s">
+        <v>73</v>
+      </c>
+      <c r="HV2" s="4" t="s">
+        <v>70</v>
+      </c>
+      <c r="HW2" s="4" t="s">
+        <v>71</v>
+      </c>
+      <c r="HX2" s="4" t="s">
+        <v>72</v>
+      </c>
+      <c r="HY2" s="4" t="s">
+        <v>73</v>
+      </c>
+      <c r="HZ2" s="4" t="s">
+        <v>70</v>
+      </c>
+      <c r="IA2" s="4" t="s">
+        <v>71</v>
+      </c>
+      <c r="IB2" s="4" t="s">
+        <v>72</v>
+      </c>
+      <c r="IC2" s="4" t="s">
+        <v>73</v>
+      </c>
+      <c r="ID2" s="4" t="s">
+        <v>70</v>
+      </c>
+      <c r="IE2" s="4" t="s">
+        <v>71</v>
+      </c>
+      <c r="IF2" s="4" t="s">
+        <v>72</v>
+      </c>
+      <c r="IG2" s="4" t="s">
+        <v>73</v>
+      </c>
+      <c r="IH2" s="4" t="s">
+        <v>70</v>
+      </c>
+      <c r="II2" s="4" t="s">
+        <v>71</v>
+      </c>
+      <c r="IJ2" s="4" t="s">
+        <v>72</v>
+      </c>
+      <c r="IK2" s="4" t="s">
+        <v>73</v>
+      </c>
+      <c r="IL2" s="4" t="s">
+        <v>70</v>
+      </c>
+      <c r="IM2" s="4" t="s">
+        <v>71</v>
+      </c>
+      <c r="IN2" s="4" t="s">
+        <v>72</v>
+      </c>
+      <c r="IO2" s="4" t="s">
+        <v>73</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="5" t="s">
-        <v>36</v>
+        <v>74</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>37</v>
+        <v>75</v>
       </c>
       <c r="C3" s="5"/>
       <c r="D3" s="5"/>
@@ -1019,7 +1893,7 @@
         <v>112</v>
       </c>
       <c r="CG3" s="7" t="n">
-        <v>621</v>
+        <v>651</v>
       </c>
       <c r="CH3" s="7" t="n">
         <v>1610</v>
@@ -1031,7 +1905,7 @@
         <v>260</v>
       </c>
       <c r="CK3" s="7" t="n">
-        <v>645</v>
+        <v>700</v>
       </c>
       <c r="CL3" s="7" t="n">
         <v>1665</v>
@@ -1043,7 +1917,7 @@
         <v>152</v>
       </c>
       <c r="CO3" s="7" t="n">
-        <v>670</v>
+        <v>749</v>
       </c>
       <c r="CP3" s="7" t="n">
         <v>1710</v>
@@ -1055,7 +1929,235 @@
         <v>250</v>
       </c>
       <c r="CS3" s="7" t="n">
-        <v>690</v>
+        <v>777</v>
+      </c>
+      <c r="CT3" s="7"/>
+      <c r="CU3" s="7"/>
+      <c r="CV3" s="7"/>
+      <c r="CW3" s="7" t="n">
+        <v>784</v>
+      </c>
+      <c r="CX3" s="7"/>
+      <c r="CY3" s="7"/>
+      <c r="CZ3" s="7"/>
+      <c r="DA3" s="7" t="n">
+        <v>791</v>
+      </c>
+      <c r="DB3" s="7"/>
+      <c r="DC3" s="7"/>
+      <c r="DD3" s="7"/>
+      <c r="DE3" s="7" t="n">
+        <v>798</v>
+      </c>
+      <c r="DF3" s="7"/>
+      <c r="DG3" s="7"/>
+      <c r="DH3" s="7"/>
+      <c r="DI3" s="7" t="n">
+        <v>805</v>
+      </c>
+      <c r="DJ3" s="7"/>
+      <c r="DK3" s="7"/>
+      <c r="DL3" s="7"/>
+      <c r="DM3" s="7" t="n">
+        <v>805</v>
+      </c>
+      <c r="DN3" s="7"/>
+      <c r="DO3" s="7"/>
+      <c r="DP3" s="7"/>
+      <c r="DQ3" s="7" t="n">
+        <v>812</v>
+      </c>
+      <c r="DR3" s="7"/>
+      <c r="DS3" s="7"/>
+      <c r="DT3" s="7"/>
+      <c r="DU3" s="7" t="n">
+        <v>812</v>
+      </c>
+      <c r="DV3" s="7"/>
+      <c r="DW3" s="7"/>
+      <c r="DX3" s="7"/>
+      <c r="DY3" s="7" t="n">
+        <v>819</v>
+      </c>
+      <c r="DZ3" s="7"/>
+      <c r="EA3" s="7"/>
+      <c r="EB3" s="7"/>
+      <c r="EC3" s="7" t="n">
+        <v>819</v>
+      </c>
+      <c r="ED3" s="7"/>
+      <c r="EE3" s="7"/>
+      <c r="EF3" s="7"/>
+      <c r="EG3" s="7" t="n">
+        <v>819</v>
+      </c>
+      <c r="EH3" s="7"/>
+      <c r="EI3" s="7"/>
+      <c r="EJ3" s="7"/>
+      <c r="EK3" s="7" t="n">
+        <v>819</v>
+      </c>
+      <c r="EL3" s="7"/>
+      <c r="EM3" s="7"/>
+      <c r="EN3" s="7"/>
+      <c r="EO3" s="7" t="n">
+        <v>819</v>
+      </c>
+      <c r="EP3" s="7"/>
+      <c r="EQ3" s="7"/>
+      <c r="ER3" s="7"/>
+      <c r="ES3" s="7" t="n">
+        <v>819</v>
+      </c>
+      <c r="ET3" s="7"/>
+      <c r="EU3" s="7"/>
+      <c r="EV3" s="7"/>
+      <c r="EW3" s="7" t="n">
+        <v>819</v>
+      </c>
+      <c r="EX3" s="7"/>
+      <c r="EY3" s="7"/>
+      <c r="EZ3" s="7"/>
+      <c r="FA3" s="7" t="n">
+        <v>819</v>
+      </c>
+      <c r="FB3" s="7"/>
+      <c r="FC3" s="7"/>
+      <c r="FD3" s="7"/>
+      <c r="FE3" s="7" t="n">
+        <v>819</v>
+      </c>
+      <c r="FF3" s="7"/>
+      <c r="FG3" s="7"/>
+      <c r="FH3" s="7"/>
+      <c r="FI3" s="7" t="n">
+        <v>819</v>
+      </c>
+      <c r="FJ3" s="7"/>
+      <c r="FK3" s="7"/>
+      <c r="FL3" s="7"/>
+      <c r="FM3" s="7" t="n">
+        <v>819</v>
+      </c>
+      <c r="FN3" s="7"/>
+      <c r="FO3" s="7"/>
+      <c r="FP3" s="7"/>
+      <c r="FQ3" s="7" t="n">
+        <v>819</v>
+      </c>
+      <c r="FR3" s="7"/>
+      <c r="FS3" s="7"/>
+      <c r="FT3" s="7"/>
+      <c r="FU3" s="7" t="n">
+        <v>819</v>
+      </c>
+      <c r="FV3" s="7"/>
+      <c r="FW3" s="7"/>
+      <c r="FX3" s="7"/>
+      <c r="FY3" s="7" t="n">
+        <v>819</v>
+      </c>
+      <c r="FZ3" s="7"/>
+      <c r="GA3" s="7"/>
+      <c r="GB3" s="7"/>
+      <c r="GC3" s="7" t="n">
+        <v>819</v>
+      </c>
+      <c r="GD3" s="7"/>
+      <c r="GE3" s="7"/>
+      <c r="GF3" s="7"/>
+      <c r="GG3" s="7" t="n">
+        <v>819</v>
+      </c>
+      <c r="GH3" s="7"/>
+      <c r="GI3" s="7"/>
+      <c r="GJ3" s="7"/>
+      <c r="GK3" s="7" t="n">
+        <v>819</v>
+      </c>
+      <c r="GL3" s="7"/>
+      <c r="GM3" s="7"/>
+      <c r="GN3" s="7"/>
+      <c r="GO3" s="7" t="n">
+        <v>819</v>
+      </c>
+      <c r="GP3" s="7"/>
+      <c r="GQ3" s="7"/>
+      <c r="GR3" s="7"/>
+      <c r="GS3" s="7" t="n">
+        <v>819</v>
+      </c>
+      <c r="GT3" s="7"/>
+      <c r="GU3" s="7"/>
+      <c r="GV3" s="7"/>
+      <c r="GW3" s="7" t="n">
+        <v>819</v>
+      </c>
+      <c r="GX3" s="7"/>
+      <c r="GY3" s="7"/>
+      <c r="GZ3" s="7"/>
+      <c r="HA3" s="7" t="n">
+        <v>819</v>
+      </c>
+      <c r="HB3" s="7"/>
+      <c r="HC3" s="7"/>
+      <c r="HD3" s="7"/>
+      <c r="HE3" s="7" t="n">
+        <v>819</v>
+      </c>
+      <c r="HF3" s="7"/>
+      <c r="HG3" s="7"/>
+      <c r="HH3" s="7"/>
+      <c r="HI3" s="7" t="n">
+        <v>819</v>
+      </c>
+      <c r="HJ3" s="7"/>
+      <c r="HK3" s="7"/>
+      <c r="HL3" s="7"/>
+      <c r="HM3" s="7" t="n">
+        <v>819</v>
+      </c>
+      <c r="HN3" s="7"/>
+      <c r="HO3" s="7"/>
+      <c r="HP3" s="7"/>
+      <c r="HQ3" s="7" t="n">
+        <v>819</v>
+      </c>
+      <c r="HR3" s="7"/>
+      <c r="HS3" s="7"/>
+      <c r="HT3" s="7"/>
+      <c r="HU3" s="7" t="n">
+        <v>819</v>
+      </c>
+      <c r="HV3" s="7"/>
+      <c r="HW3" s="7"/>
+      <c r="HX3" s="7"/>
+      <c r="HY3" s="7" t="n">
+        <v>819</v>
+      </c>
+      <c r="HZ3" s="7"/>
+      <c r="IA3" s="7"/>
+      <c r="IB3" s="7"/>
+      <c r="IC3" s="7" t="n">
+        <v>819</v>
+      </c>
+      <c r="ID3" s="7"/>
+      <c r="IE3" s="7"/>
+      <c r="IF3" s="7"/>
+      <c r="IG3" s="7" t="n">
+        <v>819</v>
+      </c>
+      <c r="IH3" s="7"/>
+      <c r="II3" s="7"/>
+      <c r="IJ3" s="7"/>
+      <c r="IK3" s="7" t="n">
+        <v>819</v>
+      </c>
+      <c r="IL3" s="7"/>
+      <c r="IM3" s="7"/>
+      <c r="IN3" s="7"/>
+      <c r="IO3" s="7" t="n">
+        <v>819</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1084,6 +2186,44 @@
       <c r="CH8" s="8"/>
       <c r="CL8" s="8"/>
       <c r="CP8" s="8"/>
+      <c r="CT8" s="8"/>
+      <c r="CX8" s="8"/>
+      <c r="DB8" s="8"/>
+      <c r="DF8" s="8"/>
+      <c r="DJ8" s="8"/>
+      <c r="DN8" s="8"/>
+      <c r="DR8" s="8"/>
+      <c r="DV8" s="8"/>
+      <c r="DZ8" s="8"/>
+      <c r="ED8" s="8"/>
+      <c r="EH8" s="8"/>
+      <c r="EL8" s="8"/>
+      <c r="EP8" s="8"/>
+      <c r="ET8" s="8"/>
+      <c r="EX8" s="8"/>
+      <c r="FB8" s="8"/>
+      <c r="FF8" s="8"/>
+      <c r="FJ8" s="8"/>
+      <c r="FN8" s="8"/>
+      <c r="FR8" s="8"/>
+      <c r="FV8" s="8"/>
+      <c r="FZ8" s="8"/>
+      <c r="GD8" s="8"/>
+      <c r="GH8" s="8"/>
+      <c r="GL8" s="8"/>
+      <c r="GP8" s="8"/>
+      <c r="GT8" s="8"/>
+      <c r="GX8" s="8"/>
+      <c r="HB8" s="8"/>
+      <c r="HF8" s="8"/>
+      <c r="HJ8" s="8"/>
+      <c r="HN8" s="8"/>
+      <c r="HR8" s="8"/>
+      <c r="HV8" s="8"/>
+      <c r="HZ8" s="8"/>
+      <c r="ID8" s="8"/>
+      <c r="IH8" s="8"/>
+      <c r="IL8" s="8"/>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="F9" s="1"/>
@@ -1186,9 +2326,165 @@
       <c r="CQ10" s="1"/>
       <c r="CR10" s="1"/>
       <c r="CS10" s="1"/>
+      <c r="CT10" s="1"/>
+      <c r="CU10" s="1"/>
+      <c r="CV10" s="1"/>
+      <c r="CW10" s="1"/>
+      <c r="CX10" s="1"/>
+      <c r="CY10" s="1"/>
+      <c r="CZ10" s="1"/>
+      <c r="DA10" s="1"/>
+      <c r="DB10" s="1"/>
+      <c r="DC10" s="1"/>
+      <c r="DD10" s="1"/>
+      <c r="DE10" s="1"/>
+      <c r="DF10" s="1"/>
+      <c r="DG10" s="1"/>
+      <c r="DH10" s="1"/>
+      <c r="DI10" s="1"/>
+      <c r="DJ10" s="1"/>
+      <c r="DK10" s="1"/>
+      <c r="DL10" s="1"/>
+      <c r="DM10" s="1"/>
+      <c r="DN10" s="1"/>
+      <c r="DO10" s="1"/>
+      <c r="DP10" s="1"/>
+      <c r="DQ10" s="1"/>
+      <c r="DR10" s="1"/>
+      <c r="DS10" s="1"/>
+      <c r="DT10" s="1"/>
+      <c r="DU10" s="1"/>
+      <c r="DV10" s="1"/>
+      <c r="DW10" s="1"/>
+      <c r="DX10" s="1"/>
+      <c r="DY10" s="1"/>
+      <c r="DZ10" s="1"/>
+      <c r="EA10" s="1"/>
+      <c r="EB10" s="1"/>
+      <c r="EC10" s="1"/>
+      <c r="ED10" s="1"/>
+      <c r="EE10" s="1"/>
+      <c r="EF10" s="1"/>
+      <c r="EG10" s="1"/>
+      <c r="EH10" s="1"/>
+      <c r="EI10" s="1"/>
+      <c r="EJ10" s="1"/>
+      <c r="EK10" s="1"/>
+      <c r="EL10" s="1"/>
+      <c r="EM10" s="1"/>
+      <c r="EN10" s="1"/>
+      <c r="EO10" s="1"/>
+      <c r="EP10" s="1"/>
+      <c r="EQ10" s="1"/>
+      <c r="ER10" s="1"/>
+      <c r="ES10" s="1"/>
+      <c r="ET10" s="1"/>
+      <c r="EU10" s="1"/>
+      <c r="EV10" s="1"/>
+      <c r="EW10" s="1"/>
+      <c r="EX10" s="1"/>
+      <c r="EY10" s="1"/>
+      <c r="EZ10" s="1"/>
+      <c r="FA10" s="1"/>
+      <c r="FB10" s="1"/>
+      <c r="FC10" s="1"/>
+      <c r="FD10" s="1"/>
+      <c r="FE10" s="1"/>
+      <c r="FF10" s="1"/>
+      <c r="FG10" s="1"/>
+      <c r="FH10" s="1"/>
+      <c r="FI10" s="1"/>
+      <c r="FJ10" s="1"/>
+      <c r="FK10" s="1"/>
+      <c r="FL10" s="1"/>
+      <c r="FM10" s="1"/>
+      <c r="FN10" s="1"/>
+      <c r="FO10" s="1"/>
+      <c r="FP10" s="1"/>
+      <c r="FQ10" s="1"/>
+      <c r="FR10" s="1"/>
+      <c r="FS10" s="1"/>
+      <c r="FT10" s="1"/>
+      <c r="FU10" s="1"/>
+      <c r="FV10" s="1"/>
+      <c r="FW10" s="1"/>
+      <c r="FX10" s="1"/>
+      <c r="FY10" s="1"/>
+      <c r="FZ10" s="1"/>
+      <c r="GA10" s="1"/>
+      <c r="GB10" s="1"/>
+      <c r="GC10" s="1"/>
+      <c r="GD10" s="1"/>
+      <c r="GE10" s="1"/>
+      <c r="GF10" s="1"/>
+      <c r="GG10" s="1"/>
+      <c r="GH10" s="1"/>
+      <c r="GI10" s="1"/>
+      <c r="GJ10" s="1"/>
+      <c r="GK10" s="1"/>
+      <c r="GL10" s="1"/>
+      <c r="GM10" s="1"/>
+      <c r="GN10" s="1"/>
+      <c r="GO10" s="1"/>
+      <c r="GP10" s="1"/>
+      <c r="GQ10" s="1"/>
+      <c r="GR10" s="1"/>
+      <c r="GS10" s="1"/>
+      <c r="GT10" s="1"/>
+      <c r="GU10" s="1"/>
+      <c r="GV10" s="1"/>
+      <c r="GW10" s="1"/>
+      <c r="GX10" s="1"/>
+      <c r="GY10" s="1"/>
+      <c r="GZ10" s="1"/>
+      <c r="HA10" s="1"/>
+      <c r="HB10" s="1"/>
+      <c r="HC10" s="1"/>
+      <c r="HD10" s="1"/>
+      <c r="HE10" s="1"/>
+      <c r="HF10" s="1"/>
+      <c r="HG10" s="1"/>
+      <c r="HH10" s="1"/>
+      <c r="HI10" s="1"/>
+      <c r="HJ10" s="1"/>
+      <c r="HK10" s="1"/>
+      <c r="HL10" s="1"/>
+      <c r="HM10" s="1"/>
+      <c r="HN10" s="1"/>
+      <c r="HO10" s="1"/>
+      <c r="HP10" s="1"/>
+      <c r="HQ10" s="1"/>
+      <c r="HR10" s="1"/>
+      <c r="HS10" s="1"/>
+      <c r="HT10" s="1"/>
+      <c r="HU10" s="1"/>
+      <c r="HV10" s="1"/>
+      <c r="HW10" s="1"/>
+      <c r="HX10" s="1"/>
+      <c r="HY10" s="1"/>
+      <c r="HZ10" s="1"/>
+      <c r="IA10" s="1"/>
+      <c r="IB10" s="1"/>
+      <c r="IC10" s="1"/>
+      <c r="ID10" s="1"/>
+      <c r="IE10" s="1"/>
+      <c r="IF10" s="1"/>
+      <c r="IG10" s="1"/>
+      <c r="IH10" s="1"/>
+      <c r="II10" s="1"/>
+      <c r="IJ10" s="1"/>
+      <c r="IK10" s="1"/>
+      <c r="IL10" s="1"/>
+      <c r="IM10" s="1"/>
+      <c r="IN10" s="1"/>
+      <c r="IO10" s="1"/>
+      <c r="IP10" s="0"/>
+      <c r="IQ10" s="0"/>
+      <c r="IR10" s="0"/>
+      <c r="IS10" s="0"/>
     </row>
   </sheetData>
-  <mergeCells count="23">
+  <mergeCells count="61">
     <mergeCell ref="A1:F1"/>
     <mergeCell ref="J1:M1"/>
     <mergeCell ref="N1:Q1"/>
@@ -1212,6 +2508,44 @@
     <mergeCell ref="CH1:CK1"/>
     <mergeCell ref="CL1:CO1"/>
     <mergeCell ref="CP1:CS1"/>
+    <mergeCell ref="CT1:CW1"/>
+    <mergeCell ref="CX1:DA1"/>
+    <mergeCell ref="DB1:DE1"/>
+    <mergeCell ref="DF1:DI1"/>
+    <mergeCell ref="DJ1:DM1"/>
+    <mergeCell ref="DN1:DQ1"/>
+    <mergeCell ref="DR1:DU1"/>
+    <mergeCell ref="DV1:DY1"/>
+    <mergeCell ref="DZ1:EC1"/>
+    <mergeCell ref="ED1:EG1"/>
+    <mergeCell ref="EH1:EK1"/>
+    <mergeCell ref="EL1:EO1"/>
+    <mergeCell ref="EP1:ES1"/>
+    <mergeCell ref="ET1:EW1"/>
+    <mergeCell ref="EX1:FA1"/>
+    <mergeCell ref="FB1:FE1"/>
+    <mergeCell ref="FF1:FI1"/>
+    <mergeCell ref="FJ1:FM1"/>
+    <mergeCell ref="FN1:FQ1"/>
+    <mergeCell ref="FR1:FU1"/>
+    <mergeCell ref="FV1:FY1"/>
+    <mergeCell ref="FZ1:GC1"/>
+    <mergeCell ref="GD1:GG1"/>
+    <mergeCell ref="GH1:GK1"/>
+    <mergeCell ref="GL1:GO1"/>
+    <mergeCell ref="GP1:GS1"/>
+    <mergeCell ref="GT1:GW1"/>
+    <mergeCell ref="GX1:HA1"/>
+    <mergeCell ref="HB1:HE1"/>
+    <mergeCell ref="HF1:HI1"/>
+    <mergeCell ref="HJ1:HM1"/>
+    <mergeCell ref="HN1:HQ1"/>
+    <mergeCell ref="HR1:HU1"/>
+    <mergeCell ref="HV1:HY1"/>
+    <mergeCell ref="HZ1:IC1"/>
+    <mergeCell ref="ID1:IG1"/>
+    <mergeCell ref="IH1:IK1"/>
+    <mergeCell ref="IL1:IO1"/>
   </mergeCells>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>

</xml_diff>

<commit_message>
fixing filter by farm
</commit_message>
<xml_diff>
--- a/bovan_brown_max.xlsx
+++ b/bovan_brown_max.xlsx
@@ -459,8 +459,8 @@
   </sheetPr>
   <dimension ref="A1:IS10"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="GV1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="HU11" activeCellId="0" sqref="HU11"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="IP1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="IZ21" activeCellId="0" sqref="IZ21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>

</xml_diff>

<commit_message>
feed offered and intake excel import
</commit_message>
<xml_diff>
--- a/bovan_brown_max.xlsx
+++ b/bovan_brown_max.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="312" uniqueCount="76">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="372" uniqueCount="77">
   <si>
     <t xml:space="preserve">Weeks</t>
   </si>
@@ -241,7 +241,10 @@
     <t xml:space="preserve">Egg Weight</t>
   </si>
   <si>
-    <t xml:space="preserve">Feed</t>
+    <t xml:space="preserve">Feed Offered</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Feed Refusal</t>
   </si>
   <si>
     <t xml:space="preserve">B-01</t>
@@ -457,10 +460,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:IS10"/>
+  <dimension ref="A1:LB10"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="IP1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="IZ21" activeCellId="0" sqref="IZ21"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="BY1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="CU3" activeCellId="0" sqref="CU3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -475,124 +478,127 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="1" width="10.2"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="1" width="7.3"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="11" style="1" width="7.18"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="14" style="1" width="7.3"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="17" min="15" style="1" width="7.18"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="18" min="18" style="1" width="7.3"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="21" min="19" style="1" width="7.18"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="22" min="22" style="1" width="7.3"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="25" min="23" style="1" width="7.18"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="26" min="26" style="1" width="7.3"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="29" min="27" style="1" width="7.18"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="15" min="14" style="1" width="7.3"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="19" min="16" style="1" width="7.18"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="20" min="20" style="1" width="7.3"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="24" min="21" style="1" width="7.18"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="25" min="25" style="1" width="7.3"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="29" min="26" style="1" width="7.18"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="30" min="30" style="1" width="7.3"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="33" min="31" style="1" width="7.18"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="34" min="34" style="1" width="7.3"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="37" min="35" style="1" width="7.18"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="38" min="38" style="1" width="7.3"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="41" min="39" style="1" width="7.18"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="42" min="42" style="1" width="7.3"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="45" min="43" style="1" width="7.18"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="46" min="46" style="1" width="7.3"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="49" min="47" style="1" width="7.18"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="34" min="31" style="1" width="7.18"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="35" min="35" style="1" width="7.3"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="39" min="36" style="1" width="7.18"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="40" min="40" style="1" width="7.3"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="44" min="41" style="1" width="7.18"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="45" min="45" style="1" width="7.3"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="49" min="46" style="1" width="7.18"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="50" min="50" style="1" width="7.3"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="53" min="51" style="1" width="7.18"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="54" min="54" style="1" width="7.3"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="57" min="55" style="1" width="7.18"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="58" min="58" style="1" width="7.3"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="61" min="59" style="1" width="7.18"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="62" min="62" style="1" width="7.3"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="65" min="63" style="1" width="7.18"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="66" min="66" style="1" width="7.3"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="69" min="67" style="1" width="7.18"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="54" min="51" style="1" width="7.18"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="55" min="55" style="1" width="7.3"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="59" min="56" style="1" width="7.18"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="60" min="60" style="1" width="7.3"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="64" min="61" style="1" width="7.18"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="65" min="65" style="1" width="7.3"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="69" min="66" style="1" width="7.18"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="70" min="70" style="1" width="7.3"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="73" min="71" style="1" width="7.18"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="74" min="74" style="1" width="7.3"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="77" min="75" style="1" width="7.18"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="78" min="78" style="1" width="7.3"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="81" min="79" style="1" width="7.18"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="82" min="82" style="1" width="7.3"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="85" min="83" style="1" width="7.18"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="86" min="86" style="1" width="7.3"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="89" min="87" style="1" width="7.18"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="74" min="71" style="1" width="7.18"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="75" min="75" style="1" width="7.3"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="79" min="76" style="1" width="7.18"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="80" min="80" style="1" width="7.3"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="84" min="81" style="1" width="7.18"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="85" min="85" style="1" width="7.3"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="89" min="86" style="1" width="7.18"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="90" min="90" style="1" width="7.3"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="93" min="91" style="1" width="7.18"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="94" min="94" style="1" width="7.3"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="97" min="95" style="1" width="7.18"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="98" min="98" style="1" width="7.3"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="101" min="99" style="1" width="7.18"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="102" min="102" style="1" width="7.3"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="105" min="103" style="1" width="7.18"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="106" min="106" style="1" width="7.3"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="109" min="107" style="1" width="7.18"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="94" min="91" style="1" width="7.18"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="95" min="95" style="1" width="7.3"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="99" min="96" style="1" width="7.18"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="100" min="100" style="1" width="7.3"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="104" min="101" style="1" width="7.18"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="105" min="105" style="1" width="7.3"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="109" min="106" style="1" width="7.18"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="110" min="110" style="1" width="7.3"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="113" min="111" style="1" width="7.18"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="114" min="114" style="1" width="7.3"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="117" min="115" style="1" width="7.18"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="118" min="118" style="1" width="7.3"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="121" min="119" style="1" width="7.18"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="122" min="122" style="1" width="7.3"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="125" min="123" style="1" width="7.18"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="126" min="126" style="1" width="7.3"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="129" min="127" style="1" width="7.18"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="114" min="111" style="1" width="7.18"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="115" min="115" style="1" width="7.3"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="119" min="116" style="1" width="7.18"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="120" min="120" style="1" width="7.3"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="124" min="121" style="1" width="7.18"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="125" min="125" style="1" width="7.3"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="129" min="126" style="1" width="7.18"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="130" min="130" style="1" width="7.3"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="133" min="131" style="1" width="7.18"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="134" min="134" style="1" width="7.3"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="137" min="135" style="1" width="7.18"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="138" min="138" style="1" width="7.3"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="141" min="139" style="1" width="7.18"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="142" min="142" style="1" width="7.3"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="145" min="143" style="1" width="7.18"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="146" min="146" style="1" width="7.3"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="149" min="147" style="1" width="7.18"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="134" min="131" style="1" width="7.18"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="135" min="135" style="1" width="7.3"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="139" min="136" style="1" width="7.18"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="140" min="140" style="1" width="7.3"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="144" min="141" style="1" width="7.18"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="145" min="145" style="1" width="7.3"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="149" min="146" style="1" width="7.18"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="150" min="150" style="1" width="7.3"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="153" min="151" style="1" width="7.18"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="154" min="154" style="1" width="7.3"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="157" min="155" style="1" width="7.18"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="158" min="158" style="1" width="7.3"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="161" min="159" style="1" width="7.18"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="162" min="162" style="1" width="7.3"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="165" min="163" style="1" width="7.18"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="166" min="166" style="1" width="7.3"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="169" min="167" style="1" width="7.18"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="154" min="151" style="1" width="7.18"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="155" min="155" style="1" width="7.3"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="159" min="156" style="1" width="7.18"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="160" min="160" style="1" width="7.3"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="164" min="161" style="1" width="7.18"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="165" min="165" style="1" width="7.3"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="169" min="166" style="1" width="7.18"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="170" min="170" style="1" width="7.3"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="173" min="171" style="1" width="7.18"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="174" min="174" style="1" width="7.3"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="177" min="175" style="1" width="7.18"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="178" min="178" style="1" width="7.3"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="181" min="179" style="1" width="7.18"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="182" min="182" style="1" width="7.3"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="185" min="183" style="1" width="7.18"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="186" min="186" style="1" width="7.3"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="189" min="187" style="1" width="7.18"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="174" min="171" style="1" width="7.18"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="175" min="175" style="1" width="7.3"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="179" min="176" style="1" width="7.18"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="180" min="180" style="1" width="7.3"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="181" min="181" style="1" width="7.18"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="182" min="182" style="1" width="12.93"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="183" min="183" style="1" width="14.18"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="184" min="184" style="1" width="7.18"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="185" min="185" style="1" width="7.3"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="189" min="186" style="1" width="7.18"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="190" min="190" style="1" width="7.3"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="193" min="191" style="1" width="7.18"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="194" min="194" style="1" width="7.3"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="197" min="195" style="1" width="7.18"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="198" min="198" style="1" width="7.3"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="201" min="199" style="1" width="7.18"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="202" min="202" style="1" width="7.3"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="205" min="203" style="1" width="7.18"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="206" min="206" style="1" width="7.3"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="209" min="207" style="1" width="7.18"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="194" min="191" style="1" width="7.18"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="195" min="195" style="1" width="7.3"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="199" min="196" style="1" width="7.18"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="200" min="200" style="1" width="7.3"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="204" min="201" style="1" width="7.18"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="205" min="205" style="1" width="7.3"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="209" min="206" style="1" width="7.18"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="210" min="210" style="1" width="7.3"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="213" min="211" style="1" width="7.18"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="214" min="214" style="1" width="7.3"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="217" min="215" style="1" width="7.18"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="218" min="218" style="1" width="7.3"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="221" min="219" style="1" width="7.18"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="222" min="222" style="1" width="7.3"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="225" min="223" style="1" width="7.18"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="226" min="226" style="1" width="7.3"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="229" min="227" style="1" width="7.18"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="214" min="211" style="1" width="7.18"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="215" min="215" style="1" width="7.3"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="219" min="216" style="1" width="7.18"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="220" min="220" style="1" width="7.3"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="224" min="221" style="1" width="7.18"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="225" min="225" style="1" width="7.3"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="229" min="226" style="1" width="7.18"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="230" min="230" style="1" width="7.3"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="233" min="231" style="1" width="7.18"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="234" min="234" style="1" width="7.3"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="237" min="235" style="1" width="7.18"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="238" min="238" style="1" width="7.3"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="241" min="239" style="1" width="7.18"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="242" min="242" style="1" width="7.3"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="245" min="243" style="1" width="7.18"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="246" min="246" style="1" width="7.3"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="249" min="247" style="1" width="7.18"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="234" min="231" style="1" width="7.18"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="235" min="235" style="1" width="7.3"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="239" min="236" style="1" width="7.18"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="240" min="240" style="1" width="7.3"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="244" min="241" style="1" width="7.18"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="245" min="245" style="1" width="7.3"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="249" min="246" style="1" width="7.18"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="250" min="250" style="1" width="7.3"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="254" min="251" style="1" width="7.18"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="255" min="255" style="1" width="7.3"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="259" min="256" style="1" width="7.18"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="260" min="260" style="1" width="7.3"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="264" min="261" style="1" width="7.18"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="265" min="265" style="1" width="7.3"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="269" min="266" style="1" width="7.18"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="270" min="270" style="1" width="7.3"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="274" min="271" style="1" width="7.18"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="275" min="275" style="1" width="7.3"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="279" min="276" style="1" width="7.18"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="280" min="280" style="1" width="7.3"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="284" min="281" style="1" width="7.18"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="285" min="285" style="1" width="7.3"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="289" min="286" style="1" width="7.18"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="290" min="290" style="1" width="7.3"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="294" min="291" style="1" width="7.18"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="295" min="295" style="1" width="7.3"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="299" min="296" style="1" width="7.18"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="300" min="300" style="1" width="7.3"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="304" min="301" style="1" width="7.18"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="305" min="305" style="1" width="7.3"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="309" min="306" style="1" width="7.18"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="29.85" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -613,360 +619,420 @@
       <c r="K1" s="3"/>
       <c r="L1" s="3"/>
       <c r="M1" s="3"/>
-      <c r="N1" s="3" t="s">
+      <c r="N1" s="3"/>
+      <c r="O1" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="O1" s="3"/>
       <c r="P1" s="3"/>
       <c r="Q1" s="3"/>
-      <c r="R1" s="3" t="s">
+      <c r="R1" s="3"/>
+      <c r="S1" s="3"/>
+      <c r="T1" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="S1" s="3"/>
-      <c r="T1" s="3"/>
       <c r="U1" s="3"/>
-      <c r="V1" s="3" t="s">
-        <v>4</v>
-      </c>
+      <c r="V1" s="3"/>
       <c r="W1" s="3"/>
       <c r="X1" s="3"/>
-      <c r="Y1" s="3"/>
-      <c r="Z1" s="3" t="s">
-        <v>5</v>
-      </c>
+      <c r="Y1" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="Z1" s="3"/>
       <c r="AA1" s="3"/>
       <c r="AB1" s="3"/>
       <c r="AC1" s="3"/>
       <c r="AD1" s="3" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="AE1" s="3"/>
       <c r="AF1" s="3"/>
       <c r="AG1" s="3"/>
-      <c r="AH1" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="AI1" s="3"/>
+      <c r="AH1" s="3"/>
+      <c r="AI1" s="3" t="s">
+        <v>6</v>
+      </c>
       <c r="AJ1" s="3"/>
       <c r="AK1" s="3"/>
-      <c r="AL1" s="3" t="s">
-        <v>8</v>
-      </c>
+      <c r="AL1" s="3"/>
       <c r="AM1" s="3"/>
-      <c r="AN1" s="3"/>
+      <c r="AN1" s="3" t="s">
+        <v>7</v>
+      </c>
       <c r="AO1" s="3"/>
-      <c r="AP1" s="3" t="s">
-        <v>9</v>
-      </c>
+      <c r="AP1" s="3"/>
       <c r="AQ1" s="3"/>
       <c r="AR1" s="3"/>
-      <c r="AS1" s="3"/>
-      <c r="AT1" s="3" t="s">
-        <v>10</v>
-      </c>
+      <c r="AS1" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="AT1" s="3"/>
       <c r="AU1" s="3"/>
       <c r="AV1" s="3"/>
       <c r="AW1" s="3"/>
       <c r="AX1" s="3" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="AY1" s="3"/>
       <c r="AZ1" s="3"/>
       <c r="BA1" s="3"/>
-      <c r="BB1" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="BC1" s="3"/>
+      <c r="BB1" s="3"/>
+      <c r="BC1" s="3" t="s">
+        <v>10</v>
+      </c>
       <c r="BD1" s="3"/>
       <c r="BE1" s="3"/>
-      <c r="BF1" s="3" t="s">
-        <v>13</v>
-      </c>
+      <c r="BF1" s="3"/>
       <c r="BG1" s="3"/>
-      <c r="BH1" s="3"/>
+      <c r="BH1" s="3" t="s">
+        <v>11</v>
+      </c>
       <c r="BI1" s="3"/>
-      <c r="BJ1" s="3" t="s">
-        <v>14</v>
-      </c>
+      <c r="BJ1" s="3"/>
       <c r="BK1" s="3"/>
       <c r="BL1" s="3"/>
-      <c r="BM1" s="3"/>
-      <c r="BN1" s="3" t="s">
-        <v>15</v>
-      </c>
+      <c r="BM1" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="BN1" s="3"/>
       <c r="BO1" s="3"/>
       <c r="BP1" s="3"/>
       <c r="BQ1" s="3"/>
       <c r="BR1" s="3" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="BS1" s="3"/>
       <c r="BT1" s="3"/>
       <c r="BU1" s="3"/>
-      <c r="BV1" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="BW1" s="3"/>
+      <c r="BV1" s="3"/>
+      <c r="BW1" s="3" t="s">
+        <v>14</v>
+      </c>
       <c r="BX1" s="3"/>
       <c r="BY1" s="3"/>
-      <c r="BZ1" s="3" t="s">
-        <v>18</v>
-      </c>
+      <c r="BZ1" s="3"/>
       <c r="CA1" s="3"/>
-      <c r="CB1" s="3"/>
+      <c r="CB1" s="3" t="s">
+        <v>15</v>
+      </c>
       <c r="CC1" s="3"/>
-      <c r="CD1" s="3" t="s">
-        <v>19</v>
-      </c>
+      <c r="CD1" s="3"/>
       <c r="CE1" s="3"/>
       <c r="CF1" s="3"/>
-      <c r="CG1" s="3"/>
-      <c r="CH1" s="3" t="s">
-        <v>20</v>
-      </c>
+      <c r="CG1" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="CH1" s="3"/>
       <c r="CI1" s="3"/>
       <c r="CJ1" s="3"/>
       <c r="CK1" s="3"/>
       <c r="CL1" s="3" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="CM1" s="3"/>
       <c r="CN1" s="3"/>
       <c r="CO1" s="3"/>
-      <c r="CP1" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="CQ1" s="3"/>
+      <c r="CP1" s="3"/>
+      <c r="CQ1" s="3" t="s">
+        <v>18</v>
+      </c>
       <c r="CR1" s="3"/>
       <c r="CS1" s="3"/>
-      <c r="CT1" s="3" t="s">
-        <v>23</v>
-      </c>
+      <c r="CT1" s="3"/>
       <c r="CU1" s="3"/>
-      <c r="CV1" s="3"/>
+      <c r="CV1" s="3" t="s">
+        <v>19</v>
+      </c>
       <c r="CW1" s="3"/>
-      <c r="CX1" s="3" t="s">
-        <v>24</v>
-      </c>
+      <c r="CX1" s="3"/>
       <c r="CY1" s="3"/>
       <c r="CZ1" s="3"/>
-      <c r="DA1" s="3"/>
-      <c r="DB1" s="3" t="s">
-        <v>25</v>
-      </c>
+      <c r="DA1" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="DB1" s="3"/>
       <c r="DC1" s="3"/>
       <c r="DD1" s="3"/>
       <c r="DE1" s="3"/>
       <c r="DF1" s="3" t="s">
-        <v>26</v>
+        <v>21</v>
       </c>
       <c r="DG1" s="3"/>
       <c r="DH1" s="3"/>
       <c r="DI1" s="3"/>
-      <c r="DJ1" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="DK1" s="3"/>
+      <c r="DJ1" s="3"/>
+      <c r="DK1" s="3" t="s">
+        <v>22</v>
+      </c>
       <c r="DL1" s="3"/>
       <c r="DM1" s="3"/>
-      <c r="DN1" s="3" t="s">
-        <v>28</v>
-      </c>
+      <c r="DN1" s="3"/>
       <c r="DO1" s="3"/>
-      <c r="DP1" s="3"/>
+      <c r="DP1" s="3" t="s">
+        <v>23</v>
+      </c>
       <c r="DQ1" s="3"/>
-      <c r="DR1" s="3" t="s">
-        <v>29</v>
-      </c>
+      <c r="DR1" s="3"/>
       <c r="DS1" s="3"/>
       <c r="DT1" s="3"/>
-      <c r="DU1" s="3"/>
-      <c r="DV1" s="3" t="s">
-        <v>30</v>
-      </c>
+      <c r="DU1" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="DV1" s="3"/>
       <c r="DW1" s="3"/>
       <c r="DX1" s="3"/>
       <c r="DY1" s="3"/>
       <c r="DZ1" s="3" t="s">
-        <v>31</v>
+        <v>25</v>
       </c>
       <c r="EA1" s="3"/>
       <c r="EB1" s="3"/>
       <c r="EC1" s="3"/>
-      <c r="ED1" s="3" t="s">
-        <v>32</v>
-      </c>
-      <c r="EE1" s="3"/>
+      <c r="ED1" s="3"/>
+      <c r="EE1" s="3" t="s">
+        <v>26</v>
+      </c>
       <c r="EF1" s="3"/>
       <c r="EG1" s="3"/>
-      <c r="EH1" s="3" t="s">
-        <v>33</v>
-      </c>
+      <c r="EH1" s="3"/>
       <c r="EI1" s="3"/>
-      <c r="EJ1" s="3"/>
+      <c r="EJ1" s="3" t="s">
+        <v>27</v>
+      </c>
       <c r="EK1" s="3"/>
-      <c r="EL1" s="3" t="s">
-        <v>34</v>
-      </c>
+      <c r="EL1" s="3"/>
       <c r="EM1" s="3"/>
       <c r="EN1" s="3"/>
-      <c r="EO1" s="3"/>
-      <c r="EP1" s="3" t="s">
-        <v>35</v>
-      </c>
+      <c r="EO1" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="EP1" s="3"/>
       <c r="EQ1" s="3"/>
       <c r="ER1" s="3"/>
       <c r="ES1" s="3"/>
       <c r="ET1" s="3" t="s">
-        <v>36</v>
+        <v>29</v>
       </c>
       <c r="EU1" s="3"/>
       <c r="EV1" s="3"/>
       <c r="EW1" s="3"/>
-      <c r="EX1" s="3" t="s">
-        <v>37</v>
-      </c>
-      <c r="EY1" s="3"/>
+      <c r="EX1" s="3"/>
+      <c r="EY1" s="3" t="s">
+        <v>30</v>
+      </c>
       <c r="EZ1" s="3"/>
       <c r="FA1" s="3"/>
-      <c r="FB1" s="3" t="s">
-        <v>38</v>
-      </c>
+      <c r="FB1" s="3"/>
       <c r="FC1" s="3"/>
-      <c r="FD1" s="3"/>
+      <c r="FD1" s="3" t="s">
+        <v>31</v>
+      </c>
       <c r="FE1" s="3"/>
-      <c r="FF1" s="3" t="s">
-        <v>39</v>
-      </c>
+      <c r="FF1" s="3"/>
       <c r="FG1" s="3"/>
       <c r="FH1" s="3"/>
-      <c r="FI1" s="3"/>
-      <c r="FJ1" s="3" t="s">
-        <v>40</v>
-      </c>
+      <c r="FI1" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="FJ1" s="3"/>
       <c r="FK1" s="3"/>
       <c r="FL1" s="3"/>
       <c r="FM1" s="3"/>
       <c r="FN1" s="3" t="s">
-        <v>41</v>
+        <v>33</v>
       </c>
       <c r="FO1" s="3"/>
       <c r="FP1" s="3"/>
       <c r="FQ1" s="3"/>
-      <c r="FR1" s="3" t="s">
-        <v>42</v>
-      </c>
-      <c r="FS1" s="3"/>
+      <c r="FR1" s="3"/>
+      <c r="FS1" s="3" t="s">
+        <v>34</v>
+      </c>
       <c r="FT1" s="3"/>
       <c r="FU1" s="3"/>
-      <c r="FV1" s="3" t="s">
-        <v>43</v>
-      </c>
+      <c r="FV1" s="3"/>
       <c r="FW1" s="3"/>
-      <c r="FX1" s="3"/>
+      <c r="FX1" s="3" t="s">
+        <v>35</v>
+      </c>
       <c r="FY1" s="3"/>
-      <c r="FZ1" s="3" t="s">
-        <v>44</v>
-      </c>
+      <c r="FZ1" s="3"/>
       <c r="GA1" s="3"/>
       <c r="GB1" s="3"/>
-      <c r="GC1" s="3"/>
-      <c r="GD1" s="3" t="s">
-        <v>45</v>
-      </c>
+      <c r="GC1" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="GD1" s="3"/>
       <c r="GE1" s="3"/>
       <c r="GF1" s="3"/>
       <c r="GG1" s="3"/>
       <c r="GH1" s="3" t="s">
-        <v>46</v>
+        <v>37</v>
       </c>
       <c r="GI1" s="3"/>
       <c r="GJ1" s="3"/>
       <c r="GK1" s="3"/>
-      <c r="GL1" s="3" t="s">
-        <v>47</v>
-      </c>
-      <c r="GM1" s="3"/>
+      <c r="GL1" s="3"/>
+      <c r="GM1" s="3" t="s">
+        <v>38</v>
+      </c>
       <c r="GN1" s="3"/>
       <c r="GO1" s="3"/>
-      <c r="GP1" s="3" t="s">
-        <v>48</v>
-      </c>
+      <c r="GP1" s="3"/>
       <c r="GQ1" s="3"/>
-      <c r="GR1" s="3"/>
+      <c r="GR1" s="3" t="s">
+        <v>39</v>
+      </c>
       <c r="GS1" s="3"/>
-      <c r="GT1" s="3" t="s">
-        <v>49</v>
-      </c>
+      <c r="GT1" s="3"/>
       <c r="GU1" s="3"/>
       <c r="GV1" s="3"/>
-      <c r="GW1" s="3"/>
-      <c r="GX1" s="3" t="s">
-        <v>50</v>
-      </c>
+      <c r="GW1" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="GX1" s="3"/>
       <c r="GY1" s="3"/>
       <c r="GZ1" s="3"/>
       <c r="HA1" s="3"/>
       <c r="HB1" s="3" t="s">
-        <v>51</v>
+        <v>41</v>
       </c>
       <c r="HC1" s="3"/>
       <c r="HD1" s="3"/>
       <c r="HE1" s="3"/>
-      <c r="HF1" s="3" t="s">
-        <v>52</v>
-      </c>
-      <c r="HG1" s="3"/>
+      <c r="HF1" s="3"/>
+      <c r="HG1" s="3" t="s">
+        <v>42</v>
+      </c>
       <c r="HH1" s="3"/>
       <c r="HI1" s="3"/>
-      <c r="HJ1" s="3" t="s">
-        <v>53</v>
-      </c>
+      <c r="HJ1" s="3"/>
       <c r="HK1" s="3"/>
-      <c r="HL1" s="3"/>
+      <c r="HL1" s="3" t="s">
+        <v>43</v>
+      </c>
       <c r="HM1" s="3"/>
-      <c r="HN1" s="3" t="s">
-        <v>54</v>
-      </c>
+      <c r="HN1" s="3"/>
       <c r="HO1" s="3"/>
       <c r="HP1" s="3"/>
-      <c r="HQ1" s="3"/>
-      <c r="HR1" s="3" t="s">
-        <v>55</v>
-      </c>
+      <c r="HQ1" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="HR1" s="3"/>
       <c r="HS1" s="3"/>
       <c r="HT1" s="3"/>
       <c r="HU1" s="3"/>
       <c r="HV1" s="3" t="s">
-        <v>56</v>
+        <v>45</v>
       </c>
       <c r="HW1" s="3"/>
       <c r="HX1" s="3"/>
       <c r="HY1" s="3"/>
-      <c r="HZ1" s="3" t="s">
-        <v>57</v>
-      </c>
-      <c r="IA1" s="3"/>
+      <c r="HZ1" s="3"/>
+      <c r="IA1" s="3" t="s">
+        <v>46</v>
+      </c>
       <c r="IB1" s="3"/>
       <c r="IC1" s="3"/>
-      <c r="ID1" s="3" t="s">
-        <v>58</v>
-      </c>
+      <c r="ID1" s="3"/>
       <c r="IE1" s="3"/>
-      <c r="IF1" s="3"/>
+      <c r="IF1" s="3" t="s">
+        <v>47</v>
+      </c>
       <c r="IG1" s="3"/>
-      <c r="IH1" s="3" t="s">
-        <v>59</v>
-      </c>
+      <c r="IH1" s="3"/>
       <c r="II1" s="3"/>
       <c r="IJ1" s="3"/>
-      <c r="IK1" s="3"/>
-      <c r="IL1" s="3" t="s">
-        <v>60</v>
-      </c>
+      <c r="IK1" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="IL1" s="3"/>
       <c r="IM1" s="3"/>
       <c r="IN1" s="3"/>
       <c r="IO1" s="3"/>
+      <c r="IP1" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="IQ1" s="3"/>
+      <c r="IR1" s="3"/>
+      <c r="IS1" s="3"/>
+      <c r="IT1" s="3"/>
+      <c r="IU1" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="IV1" s="3"/>
+      <c r="IW1" s="3"/>
+      <c r="IX1" s="3"/>
+      <c r="IY1" s="3"/>
+      <c r="IZ1" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="JA1" s="3"/>
+      <c r="JB1" s="3"/>
+      <c r="JC1" s="3"/>
+      <c r="JD1" s="3"/>
+      <c r="JE1" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="JF1" s="3"/>
+      <c r="JG1" s="3"/>
+      <c r="JH1" s="3"/>
+      <c r="JI1" s="3"/>
+      <c r="JJ1" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="JK1" s="3"/>
+      <c r="JL1" s="3"/>
+      <c r="JM1" s="3"/>
+      <c r="JN1" s="3"/>
+      <c r="JO1" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="JP1" s="3"/>
+      <c r="JQ1" s="3"/>
+      <c r="JR1" s="3"/>
+      <c r="JS1" s="3"/>
+      <c r="JT1" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="JU1" s="3"/>
+      <c r="JV1" s="3"/>
+      <c r="JW1" s="3"/>
+      <c r="JX1" s="3"/>
+      <c r="JY1" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="JZ1" s="3"/>
+      <c r="KA1" s="3"/>
+      <c r="KB1" s="3"/>
+      <c r="KC1" s="3"/>
+      <c r="KD1" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="KE1" s="3"/>
+      <c r="KF1" s="3"/>
+      <c r="KG1" s="3"/>
+      <c r="KH1" s="3"/>
+      <c r="KI1" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="KJ1" s="3"/>
+      <c r="KK1" s="3"/>
+      <c r="KL1" s="3"/>
+      <c r="KM1" s="3"/>
+      <c r="KN1" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="KO1" s="3"/>
+      <c r="KP1" s="3"/>
+      <c r="KQ1" s="3"/>
+      <c r="KR1" s="3"/>
+      <c r="KS1" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="KT1" s="3"/>
+      <c r="KU1" s="3"/>
+      <c r="KV1" s="3"/>
+      <c r="KW1" s="3"/>
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="4" t="s">
@@ -1009,52 +1075,52 @@
         <v>73</v>
       </c>
       <c r="N2" s="4" t="s">
-        <v>70</v>
+        <v>74</v>
       </c>
       <c r="O2" s="4" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="P2" s="4" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="Q2" s="4" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="R2" s="4" t="s">
-        <v>70</v>
+        <v>73</v>
       </c>
       <c r="S2" s="4" t="s">
-        <v>71</v>
+        <v>74</v>
       </c>
       <c r="T2" s="4" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="U2" s="4" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="V2" s="4" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="W2" s="4" t="s">
-        <v>71</v>
+        <v>73</v>
       </c>
       <c r="X2" s="4" t="s">
-        <v>72</v>
+        <v>74</v>
       </c>
       <c r="Y2" s="4" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="Z2" s="4" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="AA2" s="4" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="AB2" s="4" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="AC2" s="4" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="AD2" s="4" t="s">
         <v>70</v>
@@ -1069,52 +1135,52 @@
         <v>73</v>
       </c>
       <c r="AH2" s="4" t="s">
-        <v>70</v>
+        <v>74</v>
       </c>
       <c r="AI2" s="4" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="AJ2" s="4" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="AK2" s="4" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="AL2" s="4" t="s">
-        <v>70</v>
+        <v>73</v>
       </c>
       <c r="AM2" s="4" t="s">
-        <v>71</v>
+        <v>74</v>
       </c>
       <c r="AN2" s="4" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="AO2" s="4" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="AP2" s="4" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="AQ2" s="4" t="s">
-        <v>71</v>
+        <v>73</v>
       </c>
       <c r="AR2" s="4" t="s">
-        <v>72</v>
+        <v>74</v>
       </c>
       <c r="AS2" s="4" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="AT2" s="4" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="AU2" s="4" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="AV2" s="4" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="AW2" s="4" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="AX2" s="4" t="s">
         <v>70</v>
@@ -1129,52 +1195,52 @@
         <v>73</v>
       </c>
       <c r="BB2" s="4" t="s">
-        <v>70</v>
+        <v>74</v>
       </c>
       <c r="BC2" s="4" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="BD2" s="4" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="BE2" s="4" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="BF2" s="4" t="s">
-        <v>70</v>
+        <v>73</v>
       </c>
       <c r="BG2" s="4" t="s">
-        <v>71</v>
+        <v>74</v>
       </c>
       <c r="BH2" s="4" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="BI2" s="4" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="BJ2" s="4" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="BK2" s="4" t="s">
-        <v>71</v>
+        <v>73</v>
       </c>
       <c r="BL2" s="4" t="s">
-        <v>72</v>
+        <v>74</v>
       </c>
       <c r="BM2" s="4" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="BN2" s="4" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="BO2" s="4" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="BP2" s="4" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="BQ2" s="4" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="BR2" s="4" t="s">
         <v>70</v>
@@ -1189,52 +1255,52 @@
         <v>73</v>
       </c>
       <c r="BV2" s="4" t="s">
-        <v>70</v>
+        <v>74</v>
       </c>
       <c r="BW2" s="4" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="BX2" s="4" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="BY2" s="4" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="BZ2" s="4" t="s">
-        <v>70</v>
+        <v>73</v>
       </c>
       <c r="CA2" s="4" t="s">
-        <v>71</v>
+        <v>74</v>
       </c>
       <c r="CB2" s="4" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="CC2" s="4" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="CD2" s="4" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="CE2" s="4" t="s">
-        <v>71</v>
+        <v>73</v>
       </c>
       <c r="CF2" s="4" t="s">
-        <v>72</v>
+        <v>74</v>
       </c>
       <c r="CG2" s="4" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="CH2" s="4" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="CI2" s="4" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="CJ2" s="4" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="CK2" s="4" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="CL2" s="4" t="s">
         <v>70</v>
@@ -1249,52 +1315,52 @@
         <v>73</v>
       </c>
       <c r="CP2" s="4" t="s">
-        <v>70</v>
+        <v>74</v>
       </c>
       <c r="CQ2" s="4" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="CR2" s="4" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="CS2" s="4" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="CT2" s="4" t="s">
-        <v>70</v>
+        <v>73</v>
       </c>
       <c r="CU2" s="4" t="s">
-        <v>71</v>
+        <v>74</v>
       </c>
       <c r="CV2" s="4" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="CW2" s="4" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="CX2" s="4" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="CY2" s="4" t="s">
-        <v>71</v>
+        <v>73</v>
       </c>
       <c r="CZ2" s="4" t="s">
-        <v>72</v>
+        <v>74</v>
       </c>
       <c r="DA2" s="4" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="DB2" s="4" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="DC2" s="4" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="DD2" s="4" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="DE2" s="4" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="DF2" s="4" t="s">
         <v>70</v>
@@ -1309,52 +1375,52 @@
         <v>73</v>
       </c>
       <c r="DJ2" s="4" t="s">
-        <v>70</v>
+        <v>74</v>
       </c>
       <c r="DK2" s="4" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="DL2" s="4" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="DM2" s="4" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="DN2" s="4" t="s">
-        <v>70</v>
+        <v>73</v>
       </c>
       <c r="DO2" s="4" t="s">
-        <v>71</v>
+        <v>74</v>
       </c>
       <c r="DP2" s="4" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="DQ2" s="4" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="DR2" s="4" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="DS2" s="4" t="s">
-        <v>71</v>
+        <v>73</v>
       </c>
       <c r="DT2" s="4" t="s">
-        <v>72</v>
+        <v>74</v>
       </c>
       <c r="DU2" s="4" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="DV2" s="4" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="DW2" s="4" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="DX2" s="4" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="DY2" s="4" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="DZ2" s="4" t="s">
         <v>70</v>
@@ -1369,52 +1435,52 @@
         <v>73</v>
       </c>
       <c r="ED2" s="4" t="s">
-        <v>70</v>
+        <v>74</v>
       </c>
       <c r="EE2" s="4" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="EF2" s="4" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="EG2" s="4" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="EH2" s="4" t="s">
-        <v>70</v>
+        <v>73</v>
       </c>
       <c r="EI2" s="4" t="s">
-        <v>71</v>
+        <v>74</v>
       </c>
       <c r="EJ2" s="4" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="EK2" s="4" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="EL2" s="4" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="EM2" s="4" t="s">
-        <v>71</v>
+        <v>73</v>
       </c>
       <c r="EN2" s="4" t="s">
-        <v>72</v>
+        <v>74</v>
       </c>
       <c r="EO2" s="4" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="EP2" s="4" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="EQ2" s="4" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="ER2" s="4" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="ES2" s="4" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="ET2" s="4" t="s">
         <v>70</v>
@@ -1429,52 +1495,52 @@
         <v>73</v>
       </c>
       <c r="EX2" s="4" t="s">
-        <v>70</v>
+        <v>74</v>
       </c>
       <c r="EY2" s="4" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="EZ2" s="4" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="FA2" s="4" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="FB2" s="4" t="s">
-        <v>70</v>
+        <v>73</v>
       </c>
       <c r="FC2" s="4" t="s">
-        <v>71</v>
+        <v>74</v>
       </c>
       <c r="FD2" s="4" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="FE2" s="4" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="FF2" s="4" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="FG2" s="4" t="s">
-        <v>71</v>
+        <v>73</v>
       </c>
       <c r="FH2" s="4" t="s">
-        <v>72</v>
+        <v>74</v>
       </c>
       <c r="FI2" s="4" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="FJ2" s="4" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="FK2" s="4" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="FL2" s="4" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="FM2" s="4" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="FN2" s="4" t="s">
         <v>70</v>
@@ -1489,52 +1555,52 @@
         <v>73</v>
       </c>
       <c r="FR2" s="4" t="s">
-        <v>70</v>
+        <v>74</v>
       </c>
       <c r="FS2" s="4" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="FT2" s="4" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="FU2" s="4" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="FV2" s="4" t="s">
-        <v>70</v>
+        <v>73</v>
       </c>
       <c r="FW2" s="4" t="s">
-        <v>71</v>
+        <v>74</v>
       </c>
       <c r="FX2" s="4" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="FY2" s="4" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="FZ2" s="4" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="GA2" s="4" t="s">
-        <v>71</v>
+        <v>73</v>
       </c>
       <c r="GB2" s="4" t="s">
-        <v>72</v>
+        <v>74</v>
       </c>
       <c r="GC2" s="4" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="GD2" s="4" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="GE2" s="4" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="GF2" s="4" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="GG2" s="4" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="GH2" s="4" t="s">
         <v>70</v>
@@ -1549,52 +1615,52 @@
         <v>73</v>
       </c>
       <c r="GL2" s="4" t="s">
-        <v>70</v>
+        <v>74</v>
       </c>
       <c r="GM2" s="4" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="GN2" s="4" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="GO2" s="4" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="GP2" s="4" t="s">
-        <v>70</v>
+        <v>73</v>
       </c>
       <c r="GQ2" s="4" t="s">
-        <v>71</v>
+        <v>74</v>
       </c>
       <c r="GR2" s="4" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="GS2" s="4" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="GT2" s="4" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="GU2" s="4" t="s">
-        <v>71</v>
+        <v>73</v>
       </c>
       <c r="GV2" s="4" t="s">
-        <v>72</v>
+        <v>74</v>
       </c>
       <c r="GW2" s="4" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="GX2" s="4" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="GY2" s="4" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="GZ2" s="4" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="HA2" s="4" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="HB2" s="4" t="s">
         <v>70</v>
@@ -1609,52 +1675,52 @@
         <v>73</v>
       </c>
       <c r="HF2" s="4" t="s">
-        <v>70</v>
+        <v>74</v>
       </c>
       <c r="HG2" s="4" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="HH2" s="4" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="HI2" s="4" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="HJ2" s="4" t="s">
-        <v>70</v>
+        <v>73</v>
       </c>
       <c r="HK2" s="4" t="s">
-        <v>71</v>
+        <v>74</v>
       </c>
       <c r="HL2" s="4" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="HM2" s="4" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="HN2" s="4" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="HO2" s="4" t="s">
-        <v>71</v>
+        <v>73</v>
       </c>
       <c r="HP2" s="4" t="s">
-        <v>72</v>
+        <v>74</v>
       </c>
       <c r="HQ2" s="4" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="HR2" s="4" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="HS2" s="4" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="HT2" s="4" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="HU2" s="4" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="HV2" s="4" t="s">
         <v>70</v>
@@ -1669,60 +1735,240 @@
         <v>73</v>
       </c>
       <c r="HZ2" s="4" t="s">
-        <v>70</v>
+        <v>74</v>
       </c>
       <c r="IA2" s="4" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="IB2" s="4" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="IC2" s="4" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="ID2" s="4" t="s">
-        <v>70</v>
+        <v>73</v>
       </c>
       <c r="IE2" s="4" t="s">
-        <v>71</v>
+        <v>74</v>
       </c>
       <c r="IF2" s="4" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="IG2" s="4" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="IH2" s="4" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="II2" s="4" t="s">
-        <v>71</v>
+        <v>73</v>
       </c>
       <c r="IJ2" s="4" t="s">
-        <v>72</v>
+        <v>74</v>
       </c>
       <c r="IK2" s="4" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="IL2" s="4" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="IM2" s="4" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="IN2" s="4" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="IO2" s="4" t="s">
-        <v>73</v>
+        <v>74</v>
+      </c>
+      <c r="IP2" s="4" t="s">
+        <v>70</v>
+      </c>
+      <c r="IQ2" s="4" t="s">
+        <v>71</v>
+      </c>
+      <c r="IR2" s="4" t="s">
+        <v>72</v>
+      </c>
+      <c r="IS2" s="4" t="s">
+        <v>73</v>
+      </c>
+      <c r="IT2" s="4" t="s">
+        <v>74</v>
+      </c>
+      <c r="IU2" s="4" t="s">
+        <v>70</v>
+      </c>
+      <c r="IV2" s="4" t="s">
+        <v>71</v>
+      </c>
+      <c r="IW2" s="4" t="s">
+        <v>72</v>
+      </c>
+      <c r="IX2" s="4" t="s">
+        <v>73</v>
+      </c>
+      <c r="IY2" s="4" t="s">
+        <v>74</v>
+      </c>
+      <c r="IZ2" s="4" t="s">
+        <v>70</v>
+      </c>
+      <c r="JA2" s="4" t="s">
+        <v>71</v>
+      </c>
+      <c r="JB2" s="4" t="s">
+        <v>72</v>
+      </c>
+      <c r="JC2" s="4" t="s">
+        <v>73</v>
+      </c>
+      <c r="JD2" s="4" t="s">
+        <v>74</v>
+      </c>
+      <c r="JE2" s="4" t="s">
+        <v>70</v>
+      </c>
+      <c r="JF2" s="4" t="s">
+        <v>71</v>
+      </c>
+      <c r="JG2" s="4" t="s">
+        <v>72</v>
+      </c>
+      <c r="JH2" s="4" t="s">
+        <v>73</v>
+      </c>
+      <c r="JI2" s="4" t="s">
+        <v>74</v>
+      </c>
+      <c r="JJ2" s="4" t="s">
+        <v>70</v>
+      </c>
+      <c r="JK2" s="4" t="s">
+        <v>71</v>
+      </c>
+      <c r="JL2" s="4" t="s">
+        <v>72</v>
+      </c>
+      <c r="JM2" s="4" t="s">
+        <v>73</v>
+      </c>
+      <c r="JN2" s="4" t="s">
+        <v>74</v>
+      </c>
+      <c r="JO2" s="4" t="s">
+        <v>70</v>
+      </c>
+      <c r="JP2" s="4" t="s">
+        <v>71</v>
+      </c>
+      <c r="JQ2" s="4" t="s">
+        <v>72</v>
+      </c>
+      <c r="JR2" s="4" t="s">
+        <v>73</v>
+      </c>
+      <c r="JS2" s="4" t="s">
+        <v>74</v>
+      </c>
+      <c r="JT2" s="4" t="s">
+        <v>70</v>
+      </c>
+      <c r="JU2" s="4" t="s">
+        <v>71</v>
+      </c>
+      <c r="JV2" s="4" t="s">
+        <v>72</v>
+      </c>
+      <c r="JW2" s="4" t="s">
+        <v>73</v>
+      </c>
+      <c r="JX2" s="4" t="s">
+        <v>74</v>
+      </c>
+      <c r="JY2" s="4" t="s">
+        <v>70</v>
+      </c>
+      <c r="JZ2" s="4" t="s">
+        <v>71</v>
+      </c>
+      <c r="KA2" s="4" t="s">
+        <v>72</v>
+      </c>
+      <c r="KB2" s="4" t="s">
+        <v>73</v>
+      </c>
+      <c r="KC2" s="4" t="s">
+        <v>74</v>
+      </c>
+      <c r="KD2" s="4" t="s">
+        <v>70</v>
+      </c>
+      <c r="KE2" s="4" t="s">
+        <v>71</v>
+      </c>
+      <c r="KF2" s="4" t="s">
+        <v>72</v>
+      </c>
+      <c r="KG2" s="4" t="s">
+        <v>73</v>
+      </c>
+      <c r="KH2" s="4" t="s">
+        <v>74</v>
+      </c>
+      <c r="KI2" s="4" t="s">
+        <v>70</v>
+      </c>
+      <c r="KJ2" s="4" t="s">
+        <v>71</v>
+      </c>
+      <c r="KK2" s="4" t="s">
+        <v>72</v>
+      </c>
+      <c r="KL2" s="4" t="s">
+        <v>73</v>
+      </c>
+      <c r="KM2" s="4" t="s">
+        <v>74</v>
+      </c>
+      <c r="KN2" s="4" t="s">
+        <v>70</v>
+      </c>
+      <c r="KO2" s="4" t="s">
+        <v>71</v>
+      </c>
+      <c r="KP2" s="4" t="s">
+        <v>72</v>
+      </c>
+      <c r="KQ2" s="4" t="s">
+        <v>73</v>
+      </c>
+      <c r="KR2" s="4" t="s">
+        <v>74</v>
+      </c>
+      <c r="KS2" s="4" t="s">
+        <v>70</v>
+      </c>
+      <c r="KT2" s="4" t="s">
+        <v>71</v>
+      </c>
+      <c r="KU2" s="4" t="s">
+        <v>72</v>
+      </c>
+      <c r="KV2" s="4" t="s">
+        <v>73</v>
+      </c>
+      <c r="KW2" s="4" t="s">
+        <v>74</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="5" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="C3" s="5"/>
       <c r="D3" s="5"/>
@@ -1744,300 +1990,348 @@
         <v>84</v>
       </c>
       <c r="N3" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="O3" s="7" t="n">
         <v>123</v>
       </c>
-      <c r="O3" s="7"/>
       <c r="P3" s="7"/>
-      <c r="Q3" s="7" t="n">
+      <c r="Q3" s="7"/>
+      <c r="R3" s="7" t="n">
         <v>126</v>
       </c>
-      <c r="R3" s="7" t="n">
+      <c r="S3" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="T3" s="7" t="n">
         <v>179</v>
       </c>
-      <c r="S3" s="7"/>
-      <c r="T3" s="7"/>
-      <c r="U3" s="7" t="n">
+      <c r="U3" s="7"/>
+      <c r="V3" s="7"/>
+      <c r="W3" s="7" t="n">
         <v>182</v>
       </c>
-      <c r="V3" s="7" t="n">
+      <c r="X3" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="Y3" s="7" t="n">
         <v>251</v>
       </c>
-      <c r="W3" s="7"/>
-      <c r="X3" s="7"/>
-      <c r="Y3" s="7" t="n">
+      <c r="Z3" s="7"/>
+      <c r="AA3" s="7"/>
+      <c r="AB3" s="7" t="n">
         <v>231</v>
       </c>
-      <c r="Z3" s="7" t="n">
+      <c r="AC3" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="AD3" s="7" t="n">
         <v>394</v>
-      </c>
-      <c r="AA3" s="7"/>
-      <c r="AB3" s="7"/>
-      <c r="AC3" s="7" t="n">
-        <v>266</v>
-      </c>
-      <c r="AD3" s="7" t="n">
-        <v>451</v>
       </c>
       <c r="AE3" s="7"/>
       <c r="AF3" s="7"/>
       <c r="AG3" s="7" t="n">
+        <v>266</v>
+      </c>
+      <c r="AH3" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="AI3" s="7" t="n">
+        <v>451</v>
+      </c>
+      <c r="AJ3" s="7"/>
+      <c r="AK3" s="7"/>
+      <c r="AL3" s="7" t="n">
         <v>301</v>
       </c>
-      <c r="AH3" s="7" t="n">
+      <c r="AM3" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="AN3" s="7" t="n">
         <v>554</v>
       </c>
-      <c r="AI3" s="7"/>
-      <c r="AJ3" s="7"/>
-      <c r="AK3" s="7" t="n">
+      <c r="AO3" s="7"/>
+      <c r="AP3" s="7"/>
+      <c r="AQ3" s="7" t="n">
         <v>329</v>
       </c>
-      <c r="AL3" s="7" t="n">
+      <c r="AR3" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="AS3" s="7" t="n">
         <v>649</v>
       </c>
-      <c r="AM3" s="7"/>
-      <c r="AN3" s="7"/>
-      <c r="AO3" s="7" t="n">
+      <c r="AT3" s="7"/>
+      <c r="AU3" s="7"/>
+      <c r="AV3" s="7" t="n">
         <v>357</v>
       </c>
-      <c r="AP3" s="7" t="n">
+      <c r="AW3" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="AX3" s="7" t="n">
         <v>738</v>
-      </c>
-      <c r="AQ3" s="7"/>
-      <c r="AR3" s="7"/>
-      <c r="AS3" s="7" t="n">
-        <v>385</v>
-      </c>
-      <c r="AT3" s="7" t="n">
-        <v>830</v>
-      </c>
-      <c r="AU3" s="7"/>
-      <c r="AV3" s="7"/>
-      <c r="AW3" s="7" t="n">
-        <v>413</v>
-      </c>
-      <c r="AX3" s="7" t="n">
-        <v>923</v>
       </c>
       <c r="AY3" s="7"/>
       <c r="AZ3" s="7"/>
       <c r="BA3" s="7" t="n">
+        <v>385</v>
+      </c>
+      <c r="BB3" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="BC3" s="7" t="n">
+        <v>830</v>
+      </c>
+      <c r="BD3" s="7"/>
+      <c r="BE3" s="7"/>
+      <c r="BF3" s="7" t="n">
+        <v>413</v>
+      </c>
+      <c r="BG3" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="BH3" s="7" t="n">
+        <v>923</v>
+      </c>
+      <c r="BI3" s="7"/>
+      <c r="BJ3" s="7"/>
+      <c r="BK3" s="7" t="n">
         <v>434</v>
       </c>
-      <c r="BB3" s="7" t="n">
+      <c r="BL3" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="BM3" s="7" t="n">
         <v>1025</v>
       </c>
-      <c r="BC3" s="7"/>
-      <c r="BD3" s="7"/>
-      <c r="BE3" s="7" t="n">
+      <c r="BN3" s="7"/>
+      <c r="BO3" s="7"/>
+      <c r="BP3" s="7" t="n">
         <v>455</v>
       </c>
-      <c r="BF3" s="7" t="n">
+      <c r="BQ3" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="BR3" s="7" t="n">
         <v>1122</v>
-      </c>
-      <c r="BG3" s="7"/>
-      <c r="BH3" s="7"/>
-      <c r="BI3" s="7" t="n">
-        <v>476</v>
-      </c>
-      <c r="BJ3" s="7" t="n">
-        <v>1210</v>
-      </c>
-      <c r="BK3" s="7"/>
-      <c r="BL3" s="7"/>
-      <c r="BM3" s="7" t="n">
-        <v>497</v>
-      </c>
-      <c r="BN3" s="7" t="n">
-        <v>1297</v>
-      </c>
-      <c r="BO3" s="7"/>
-      <c r="BP3" s="7"/>
-      <c r="BQ3" s="7" t="n">
-        <v>518</v>
-      </c>
-      <c r="BR3" s="7" t="n">
-        <v>1384</v>
       </c>
       <c r="BS3" s="7"/>
       <c r="BT3" s="7"/>
       <c r="BU3" s="7" t="n">
+        <v>476</v>
+      </c>
+      <c r="BV3" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="BW3" s="7" t="n">
+        <v>1210</v>
+      </c>
+      <c r="BX3" s="7"/>
+      <c r="BY3" s="7"/>
+      <c r="BZ3" s="7" t="n">
+        <v>497</v>
+      </c>
+      <c r="CA3" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="CB3" s="7" t="n">
+        <v>1297</v>
+      </c>
+      <c r="CC3" s="7"/>
+      <c r="CD3" s="7"/>
+      <c r="CE3" s="7" t="n">
+        <v>518</v>
+      </c>
+      <c r="CF3" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="CG3" s="7" t="n">
+        <v>1384</v>
+      </c>
+      <c r="CH3" s="7"/>
+      <c r="CI3" s="7"/>
+      <c r="CJ3" s="7" t="n">
         <v>539</v>
       </c>
-      <c r="BV3" s="7" t="n">
+      <c r="CK3" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="CL3" s="7" t="n">
         <v>1461</v>
       </c>
-      <c r="BW3" s="7"/>
-      <c r="BX3" s="7"/>
-      <c r="BY3" s="7" t="n">
+      <c r="CM3" s="7"/>
+      <c r="CN3" s="7"/>
+      <c r="CO3" s="7" t="n">
         <v>567</v>
       </c>
-      <c r="BZ3" s="7" t="n">
+      <c r="CP3" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="CQ3" s="7" t="n">
         <v>1538</v>
       </c>
-      <c r="CA3" s="7" t="n">
+      <c r="CR3" s="7" t="n">
         <v>1</v>
       </c>
-      <c r="CB3" s="7" t="n">
+      <c r="CS3" s="7" t="n">
         <v>50</v>
       </c>
-      <c r="CC3" s="7" t="n">
+      <c r="CT3" s="7" t="n">
         <v>609</v>
       </c>
-      <c r="CD3" s="7" t="n">
+      <c r="CU3" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="CV3" s="7" t="n">
         <v>1560</v>
       </c>
-      <c r="CE3" s="7" t="n">
+      <c r="CW3" s="7" t="n">
         <v>2</v>
       </c>
-      <c r="CF3" s="7" t="n">
+      <c r="CX3" s="7" t="n">
         <v>112</v>
       </c>
-      <c r="CG3" s="7" t="n">
+      <c r="CY3" s="7" t="n">
         <v>651</v>
       </c>
-      <c r="CH3" s="7" t="n">
+      <c r="CZ3" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="DA3" s="7" t="n">
         <v>1610</v>
       </c>
-      <c r="CI3" s="7" t="n">
+      <c r="DB3" s="7" t="n">
         <v>4</v>
       </c>
-      <c r="CJ3" s="7" t="n">
+      <c r="DC3" s="7" t="n">
         <v>260</v>
       </c>
-      <c r="CK3" s="7" t="n">
+      <c r="DD3" s="7" t="n">
         <v>700</v>
       </c>
-      <c r="CL3" s="7" t="n">
+      <c r="DE3" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="DF3" s="7" t="n">
         <v>1665</v>
       </c>
-      <c r="CM3" s="7" t="n">
+      <c r="DG3" s="7" t="n">
         <v>2</v>
       </c>
-      <c r="CN3" s="7" t="n">
+      <c r="DH3" s="7" t="n">
         <v>152</v>
       </c>
-      <c r="CO3" s="7" t="n">
+      <c r="DI3" s="7" t="n">
         <v>749</v>
       </c>
-      <c r="CP3" s="7" t="n">
+      <c r="DJ3" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="DK3" s="7" t="n">
         <v>1710</v>
       </c>
-      <c r="CQ3" s="7" t="n">
+      <c r="DL3" s="7" t="n">
         <v>5</v>
       </c>
-      <c r="CR3" s="7" t="n">
+      <c r="DM3" s="7" t="n">
         <v>250</v>
       </c>
-      <c r="CS3" s="7" t="n">
+      <c r="DN3" s="7" t="n">
         <v>777</v>
       </c>
-      <c r="CT3" s="7"/>
-      <c r="CU3" s="7"/>
-      <c r="CV3" s="7"/>
-      <c r="CW3" s="7" t="n">
+      <c r="DO3" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="DP3" s="7"/>
+      <c r="DQ3" s="7"/>
+      <c r="DR3" s="7"/>
+      <c r="DS3" s="7" t="n">
         <v>784</v>
       </c>
-      <c r="CX3" s="7"/>
-      <c r="CY3" s="7"/>
-      <c r="CZ3" s="7"/>
-      <c r="DA3" s="7" t="n">
-        <v>791</v>
-      </c>
-      <c r="DB3" s="7"/>
-      <c r="DC3" s="7"/>
-      <c r="DD3" s="7"/>
-      <c r="DE3" s="7" t="n">
-        <v>798</v>
-      </c>
-      <c r="DF3" s="7"/>
-      <c r="DG3" s="7"/>
-      <c r="DH3" s="7"/>
-      <c r="DI3" s="7" t="n">
-        <v>805</v>
-      </c>
-      <c r="DJ3" s="7"/>
-      <c r="DK3" s="7"/>
-      <c r="DL3" s="7"/>
-      <c r="DM3" s="7" t="n">
-        <v>805</v>
-      </c>
-      <c r="DN3" s="7"/>
-      <c r="DO3" s="7"/>
-      <c r="DP3" s="7"/>
-      <c r="DQ3" s="7" t="n">
-        <v>812</v>
-      </c>
-      <c r="DR3" s="7"/>
-      <c r="DS3" s="7"/>
-      <c r="DT3" s="7"/>
-      <c r="DU3" s="7" t="n">
-        <v>812</v>
-      </c>
+      <c r="DT3" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="DU3" s="7"/>
       <c r="DV3" s="7"/>
       <c r="DW3" s="7"/>
-      <c r="DX3" s="7"/>
+      <c r="DX3" s="7" t="n">
+        <v>791</v>
+      </c>
       <c r="DY3" s="7" t="n">
-        <v>819</v>
+        <v>0</v>
       </c>
       <c r="DZ3" s="7"/>
       <c r="EA3" s="7"/>
       <c r="EB3" s="7"/>
       <c r="EC3" s="7" t="n">
-        <v>819</v>
-      </c>
-      <c r="ED3" s="7"/>
+        <v>798</v>
+      </c>
+      <c r="ED3" s="7" t="n">
+        <v>0</v>
+      </c>
       <c r="EE3" s="7"/>
       <c r="EF3" s="7"/>
-      <c r="EG3" s="7" t="n">
-        <v>819</v>
-      </c>
-      <c r="EH3" s="7"/>
-      <c r="EI3" s="7"/>
+      <c r="EG3" s="7"/>
+      <c r="EH3" s="7" t="n">
+        <v>805</v>
+      </c>
+      <c r="EI3" s="7" t="n">
+        <v>0</v>
+      </c>
       <c r="EJ3" s="7"/>
-      <c r="EK3" s="7" t="n">
-        <v>819</v>
-      </c>
+      <c r="EK3" s="7"/>
       <c r="EL3" s="7"/>
-      <c r="EM3" s="7"/>
-      <c r="EN3" s="7"/>
-      <c r="EO3" s="7" t="n">
-        <v>819</v>
-      </c>
+      <c r="EM3" s="7" t="n">
+        <v>805</v>
+      </c>
+      <c r="EN3" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="EO3" s="7"/>
       <c r="EP3" s="7"/>
       <c r="EQ3" s="7"/>
-      <c r="ER3" s="7"/>
+      <c r="ER3" s="7" t="n">
+        <v>812</v>
+      </c>
       <c r="ES3" s="7" t="n">
-        <v>819</v>
+        <v>0</v>
       </c>
       <c r="ET3" s="7"/>
       <c r="EU3" s="7"/>
       <c r="EV3" s="7"/>
       <c r="EW3" s="7" t="n">
-        <v>819</v>
-      </c>
-      <c r="EX3" s="7"/>
+        <v>812</v>
+      </c>
+      <c r="EX3" s="7" t="n">
+        <v>0</v>
+      </c>
       <c r="EY3" s="7"/>
       <c r="EZ3" s="7"/>
-      <c r="FA3" s="7" t="n">
+      <c r="FA3" s="7"/>
+      <c r="FB3" s="7" t="n">
         <v>819</v>
       </c>
-      <c r="FB3" s="7"/>
-      <c r="FC3" s="7"/>
+      <c r="FC3" s="7" t="n">
+        <v>0</v>
+      </c>
       <c r="FD3" s="7"/>
-      <c r="FE3" s="7" t="n">
+      <c r="FE3" s="7"/>
+      <c r="FF3" s="7"/>
+      <c r="FG3" s="7" t="n">
         <v>819</v>
       </c>
-      <c r="FF3" s="7"/>
-      <c r="FG3" s="7"/>
-      <c r="FH3" s="7"/>
-      <c r="FI3" s="7" t="n">
-        <v>819</v>
-      </c>
+      <c r="FH3" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="FI3" s="7"/>
       <c r="FJ3" s="7"/>
       <c r="FK3" s="7"/>
-      <c r="FL3" s="7"/>
+      <c r="FL3" s="7" t="n">
+        <v>819</v>
+      </c>
       <c r="FM3" s="7" t="n">
-        <v>819</v>
+        <v>0</v>
       </c>
       <c r="FN3" s="7"/>
       <c r="FO3" s="7"/>
@@ -2045,29 +2339,35 @@
       <c r="FQ3" s="7" t="n">
         <v>819</v>
       </c>
-      <c r="FR3" s="7"/>
+      <c r="FR3" s="7" t="n">
+        <v>0</v>
+      </c>
       <c r="FS3" s="7"/>
       <c r="FT3" s="7"/>
-      <c r="FU3" s="7" t="n">
+      <c r="FU3" s="7"/>
+      <c r="FV3" s="7" t="n">
         <v>819</v>
       </c>
-      <c r="FV3" s="7"/>
-      <c r="FW3" s="7"/>
+      <c r="FW3" s="7" t="n">
+        <v>0</v>
+      </c>
       <c r="FX3" s="7"/>
-      <c r="FY3" s="7" t="n">
+      <c r="FY3" s="7"/>
+      <c r="FZ3" s="7"/>
+      <c r="GA3" s="7" t="n">
         <v>819</v>
       </c>
-      <c r="FZ3" s="7"/>
-      <c r="GA3" s="7"/>
-      <c r="GB3" s="7"/>
-      <c r="GC3" s="7" t="n">
-        <v>819</v>
-      </c>
+      <c r="GB3" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="GC3" s="7"/>
       <c r="GD3" s="7"/>
       <c r="GE3" s="7"/>
-      <c r="GF3" s="7"/>
+      <c r="GF3" s="7" t="n">
+        <v>819</v>
+      </c>
       <c r="GG3" s="7" t="n">
-        <v>819</v>
+        <v>0</v>
       </c>
       <c r="GH3" s="7"/>
       <c r="GI3" s="7"/>
@@ -2075,29 +2375,35 @@
       <c r="GK3" s="7" t="n">
         <v>819</v>
       </c>
-      <c r="GL3" s="7"/>
+      <c r="GL3" s="7" t="n">
+        <v>0</v>
+      </c>
       <c r="GM3" s="7"/>
       <c r="GN3" s="7"/>
-      <c r="GO3" s="7" t="n">
+      <c r="GO3" s="7"/>
+      <c r="GP3" s="7" t="n">
         <v>819</v>
       </c>
-      <c r="GP3" s="7"/>
-      <c r="GQ3" s="7"/>
+      <c r="GQ3" s="7" t="n">
+        <v>0</v>
+      </c>
       <c r="GR3" s="7"/>
-      <c r="GS3" s="7" t="n">
+      <c r="GS3" s="7"/>
+      <c r="GT3" s="7"/>
+      <c r="GU3" s="7" t="n">
         <v>819</v>
       </c>
-      <c r="GT3" s="7"/>
-      <c r="GU3" s="7"/>
-      <c r="GV3" s="7"/>
-      <c r="GW3" s="7" t="n">
-        <v>819</v>
-      </c>
+      <c r="GV3" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="GW3" s="7"/>
       <c r="GX3" s="7"/>
       <c r="GY3" s="7"/>
-      <c r="GZ3" s="7"/>
+      <c r="GZ3" s="7" t="n">
+        <v>819</v>
+      </c>
       <c r="HA3" s="7" t="n">
-        <v>819</v>
+        <v>0</v>
       </c>
       <c r="HB3" s="7"/>
       <c r="HC3" s="7"/>
@@ -2105,29 +2411,35 @@
       <c r="HE3" s="7" t="n">
         <v>819</v>
       </c>
-      <c r="HF3" s="7"/>
+      <c r="HF3" s="7" t="n">
+        <v>0</v>
+      </c>
       <c r="HG3" s="7"/>
       <c r="HH3" s="7"/>
-      <c r="HI3" s="7" t="n">
+      <c r="HI3" s="7"/>
+      <c r="HJ3" s="7" t="n">
         <v>819</v>
       </c>
-      <c r="HJ3" s="7"/>
-      <c r="HK3" s="7"/>
+      <c r="HK3" s="7" t="n">
+        <v>0</v>
+      </c>
       <c r="HL3" s="7"/>
-      <c r="HM3" s="7" t="n">
+      <c r="HM3" s="7"/>
+      <c r="HN3" s="7"/>
+      <c r="HO3" s="7" t="n">
         <v>819</v>
       </c>
-      <c r="HN3" s="7"/>
-      <c r="HO3" s="7"/>
-      <c r="HP3" s="7"/>
-      <c r="HQ3" s="7" t="n">
-        <v>819</v>
-      </c>
+      <c r="HP3" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="HQ3" s="7"/>
       <c r="HR3" s="7"/>
       <c r="HS3" s="7"/>
-      <c r="HT3" s="7"/>
+      <c r="HT3" s="7" t="n">
+        <v>819</v>
+      </c>
       <c r="HU3" s="7" t="n">
-        <v>819</v>
+        <v>0</v>
       </c>
       <c r="HV3" s="7"/>
       <c r="HW3" s="7"/>
@@ -2135,29 +2447,143 @@
       <c r="HY3" s="7" t="n">
         <v>819</v>
       </c>
-      <c r="HZ3" s="7"/>
+      <c r="HZ3" s="7" t="n">
+        <v>0</v>
+      </c>
       <c r="IA3" s="7"/>
       <c r="IB3" s="7"/>
-      <c r="IC3" s="7" t="n">
+      <c r="IC3" s="7"/>
+      <c r="ID3" s="7" t="n">
         <v>819</v>
       </c>
-      <c r="ID3" s="7"/>
-      <c r="IE3" s="7"/>
+      <c r="IE3" s="7" t="n">
+        <v>0</v>
+      </c>
       <c r="IF3" s="7"/>
-      <c r="IG3" s="7" t="n">
+      <c r="IG3" s="7"/>
+      <c r="IH3" s="7"/>
+      <c r="II3" s="7" t="n">
         <v>819</v>
       </c>
-      <c r="IH3" s="7"/>
-      <c r="II3" s="7"/>
-      <c r="IJ3" s="7"/>
-      <c r="IK3" s="7" t="n">
-        <v>819</v>
-      </c>
+      <c r="IJ3" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="IK3" s="7"/>
       <c r="IL3" s="7"/>
       <c r="IM3" s="7"/>
-      <c r="IN3" s="7"/>
+      <c r="IN3" s="7" t="n">
+        <v>819</v>
+      </c>
       <c r="IO3" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="IP3" s="7"/>
+      <c r="IQ3" s="7"/>
+      <c r="IR3" s="7"/>
+      <c r="IS3" s="7" t="n">
         <v>819</v>
+      </c>
+      <c r="IT3" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="IU3" s="7"/>
+      <c r="IV3" s="7"/>
+      <c r="IW3" s="7"/>
+      <c r="IX3" s="7" t="n">
+        <v>819</v>
+      </c>
+      <c r="IY3" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="IZ3" s="7"/>
+      <c r="JA3" s="7"/>
+      <c r="JB3" s="7"/>
+      <c r="JC3" s="7" t="n">
+        <v>819</v>
+      </c>
+      <c r="JD3" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="JE3" s="7"/>
+      <c r="JF3" s="7"/>
+      <c r="JG3" s="7"/>
+      <c r="JH3" s="7" t="n">
+        <v>819</v>
+      </c>
+      <c r="JI3" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="JJ3" s="7"/>
+      <c r="JK3" s="7"/>
+      <c r="JL3" s="7"/>
+      <c r="JM3" s="7" t="n">
+        <v>819</v>
+      </c>
+      <c r="JN3" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="JO3" s="7"/>
+      <c r="JP3" s="7"/>
+      <c r="JQ3" s="7"/>
+      <c r="JR3" s="7" t="n">
+        <v>819</v>
+      </c>
+      <c r="JS3" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="JT3" s="7"/>
+      <c r="JU3" s="7"/>
+      <c r="JV3" s="7"/>
+      <c r="JW3" s="7" t="n">
+        <v>819</v>
+      </c>
+      <c r="JX3" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="JY3" s="7"/>
+      <c r="JZ3" s="7"/>
+      <c r="KA3" s="7"/>
+      <c r="KB3" s="7" t="n">
+        <v>819</v>
+      </c>
+      <c r="KC3" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="KD3" s="7"/>
+      <c r="KE3" s="7"/>
+      <c r="KF3" s="7"/>
+      <c r="KG3" s="7" t="n">
+        <v>819</v>
+      </c>
+      <c r="KH3" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="KI3" s="7"/>
+      <c r="KJ3" s="7"/>
+      <c r="KK3" s="7"/>
+      <c r="KL3" s="7" t="n">
+        <v>819</v>
+      </c>
+      <c r="KM3" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="KN3" s="7"/>
+      <c r="KO3" s="7"/>
+      <c r="KP3" s="7"/>
+      <c r="KQ3" s="7" t="n">
+        <v>819</v>
+      </c>
+      <c r="KR3" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="KS3" s="7"/>
+      <c r="KT3" s="7"/>
+      <c r="KU3" s="7"/>
+      <c r="KV3" s="7" t="n">
+        <v>819</v>
+      </c>
+      <c r="KW3" s="7" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2165,65 +2591,65 @@
     </row>
     <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="J8" s="8"/>
-      <c r="N8" s="8"/>
-      <c r="R8" s="8"/>
-      <c r="V8" s="8"/>
-      <c r="Z8" s="8"/>
+      <c r="O8" s="8"/>
+      <c r="T8" s="8"/>
+      <c r="Y8" s="8"/>
       <c r="AD8" s="8"/>
-      <c r="AH8" s="8"/>
-      <c r="AL8" s="8"/>
-      <c r="AP8" s="8"/>
-      <c r="AT8" s="8"/>
+      <c r="AI8" s="8"/>
+      <c r="AN8" s="8"/>
+      <c r="AS8" s="8"/>
       <c r="AX8" s="8"/>
-      <c r="BB8" s="8"/>
-      <c r="BF8" s="8"/>
-      <c r="BJ8" s="8"/>
-      <c r="BN8" s="8"/>
+      <c r="BC8" s="8"/>
+      <c r="BH8" s="8"/>
+      <c r="BM8" s="8"/>
       <c r="BR8" s="8"/>
-      <c r="BV8" s="8"/>
-      <c r="BZ8" s="8"/>
-      <c r="CD8" s="8"/>
-      <c r="CH8" s="8"/>
+      <c r="BW8" s="8"/>
+      <c r="CB8" s="8"/>
+      <c r="CG8" s="8"/>
       <c r="CL8" s="8"/>
-      <c r="CP8" s="8"/>
-      <c r="CT8" s="8"/>
-      <c r="CX8" s="8"/>
-      <c r="DB8" s="8"/>
+      <c r="CQ8" s="8"/>
+      <c r="CV8" s="8"/>
+      <c r="DA8" s="8"/>
       <c r="DF8" s="8"/>
-      <c r="DJ8" s="8"/>
-      <c r="DN8" s="8"/>
-      <c r="DR8" s="8"/>
-      <c r="DV8" s="8"/>
+      <c r="DK8" s="8"/>
+      <c r="DP8" s="8"/>
+      <c r="DU8" s="8"/>
       <c r="DZ8" s="8"/>
-      <c r="ED8" s="8"/>
-      <c r="EH8" s="8"/>
-      <c r="EL8" s="8"/>
-      <c r="EP8" s="8"/>
+      <c r="EE8" s="8"/>
+      <c r="EJ8" s="8"/>
+      <c r="EO8" s="8"/>
       <c r="ET8" s="8"/>
-      <c r="EX8" s="8"/>
-      <c r="FB8" s="8"/>
-      <c r="FF8" s="8"/>
-      <c r="FJ8" s="8"/>
+      <c r="EY8" s="8"/>
+      <c r="FD8" s="8"/>
+      <c r="FI8" s="8"/>
       <c r="FN8" s="8"/>
-      <c r="FR8" s="8"/>
-      <c r="FV8" s="8"/>
-      <c r="FZ8" s="8"/>
-      <c r="GD8" s="8"/>
+      <c r="FS8" s="8"/>
+      <c r="FX8" s="8"/>
+      <c r="GC8" s="8"/>
       <c r="GH8" s="8"/>
-      <c r="GL8" s="8"/>
-      <c r="GP8" s="8"/>
-      <c r="GT8" s="8"/>
-      <c r="GX8" s="8"/>
+      <c r="GM8" s="8"/>
+      <c r="GR8" s="8"/>
+      <c r="GW8" s="8"/>
       <c r="HB8" s="8"/>
-      <c r="HF8" s="8"/>
-      <c r="HJ8" s="8"/>
-      <c r="HN8" s="8"/>
-      <c r="HR8" s="8"/>
+      <c r="HG8" s="8"/>
+      <c r="HL8" s="8"/>
+      <c r="HQ8" s="8"/>
       <c r="HV8" s="8"/>
-      <c r="HZ8" s="8"/>
-      <c r="ID8" s="8"/>
-      <c r="IH8" s="8"/>
-      <c r="IL8" s="8"/>
+      <c r="IA8" s="8"/>
+      <c r="IF8" s="8"/>
+      <c r="IK8" s="8"/>
+      <c r="IP8" s="8"/>
+      <c r="IU8" s="8"/>
+      <c r="IZ8" s="8"/>
+      <c r="JE8" s="8"/>
+      <c r="JJ8" s="8"/>
+      <c r="JO8" s="8"/>
+      <c r="JT8" s="8"/>
+      <c r="JY8" s="8"/>
+      <c r="KD8" s="8"/>
+      <c r="KI8" s="8"/>
+      <c r="KN8" s="8"/>
+      <c r="KS8" s="8"/>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="F9" s="1"/>
@@ -2478,74 +2904,135 @@
       <c r="IM10" s="1"/>
       <c r="IN10" s="1"/>
       <c r="IO10" s="1"/>
-      <c r="IP10" s="0"/>
-      <c r="IQ10" s="0"/>
-      <c r="IR10" s="0"/>
-      <c r="IS10" s="0"/>
+      <c r="IP10" s="1"/>
+      <c r="IQ10" s="1"/>
+      <c r="IR10" s="1"/>
+      <c r="IS10" s="1"/>
+      <c r="IT10" s="1"/>
+      <c r="IU10" s="1"/>
+      <c r="IV10" s="1"/>
+      <c r="IW10" s="1"/>
+      <c r="IX10" s="1"/>
+      <c r="IY10" s="1"/>
+      <c r="IZ10" s="1"/>
+      <c r="JA10" s="1"/>
+      <c r="JB10" s="1"/>
+      <c r="JC10" s="1"/>
+      <c r="JD10" s="1"/>
+      <c r="JE10" s="1"/>
+      <c r="JF10" s="1"/>
+      <c r="JG10" s="1"/>
+      <c r="JH10" s="1"/>
+      <c r="JI10" s="1"/>
+      <c r="JJ10" s="1"/>
+      <c r="JK10" s="1"/>
+      <c r="JL10" s="1"/>
+      <c r="JM10" s="1"/>
+      <c r="JN10" s="1"/>
+      <c r="JO10" s="1"/>
+      <c r="JP10" s="1"/>
+      <c r="JQ10" s="1"/>
+      <c r="JR10" s="1"/>
+      <c r="JS10" s="1"/>
+      <c r="JT10" s="1"/>
+      <c r="JU10" s="1"/>
+      <c r="JV10" s="1"/>
+      <c r="JW10" s="1"/>
+      <c r="JX10" s="1"/>
+      <c r="JY10" s="1"/>
+      <c r="JZ10" s="1"/>
+      <c r="KA10" s="1"/>
+      <c r="KB10" s="1"/>
+      <c r="KC10" s="1"/>
+      <c r="KD10" s="1"/>
+      <c r="KE10" s="1"/>
+      <c r="KF10" s="1"/>
+      <c r="KG10" s="1"/>
+      <c r="KH10" s="1"/>
+      <c r="KI10" s="1"/>
+      <c r="KJ10" s="1"/>
+      <c r="KK10" s="1"/>
+      <c r="KL10" s="1"/>
+      <c r="KM10" s="1"/>
+      <c r="KN10" s="1"/>
+      <c r="KO10" s="1"/>
+      <c r="KP10" s="1"/>
+      <c r="KQ10" s="1"/>
+      <c r="KR10" s="1"/>
+      <c r="KS10" s="1"/>
+      <c r="KT10" s="1"/>
+      <c r="KU10" s="1"/>
+      <c r="KV10" s="1"/>
+      <c r="KW10" s="1"/>
+      <c r="KX10" s="0"/>
+      <c r="KY10" s="0"/>
+      <c r="KZ10" s="0"/>
+      <c r="LA10" s="0"/>
+      <c r="LB10" s="0"/>
     </row>
   </sheetData>
   <mergeCells count="61">
     <mergeCell ref="A1:F1"/>
-    <mergeCell ref="J1:M1"/>
-    <mergeCell ref="N1:Q1"/>
-    <mergeCell ref="R1:U1"/>
-    <mergeCell ref="V1:Y1"/>
-    <mergeCell ref="Z1:AC1"/>
-    <mergeCell ref="AD1:AG1"/>
-    <mergeCell ref="AH1:AK1"/>
-    <mergeCell ref="AL1:AO1"/>
-    <mergeCell ref="AP1:AS1"/>
-    <mergeCell ref="AT1:AW1"/>
-    <mergeCell ref="AX1:BA1"/>
-    <mergeCell ref="BB1:BE1"/>
-    <mergeCell ref="BF1:BI1"/>
-    <mergeCell ref="BJ1:BM1"/>
-    <mergeCell ref="BN1:BQ1"/>
-    <mergeCell ref="BR1:BU1"/>
-    <mergeCell ref="BV1:BY1"/>
-    <mergeCell ref="BZ1:CC1"/>
-    <mergeCell ref="CD1:CG1"/>
-    <mergeCell ref="CH1:CK1"/>
-    <mergeCell ref="CL1:CO1"/>
-    <mergeCell ref="CP1:CS1"/>
-    <mergeCell ref="CT1:CW1"/>
-    <mergeCell ref="CX1:DA1"/>
-    <mergeCell ref="DB1:DE1"/>
-    <mergeCell ref="DF1:DI1"/>
-    <mergeCell ref="DJ1:DM1"/>
-    <mergeCell ref="DN1:DQ1"/>
-    <mergeCell ref="DR1:DU1"/>
-    <mergeCell ref="DV1:DY1"/>
-    <mergeCell ref="DZ1:EC1"/>
-    <mergeCell ref="ED1:EG1"/>
-    <mergeCell ref="EH1:EK1"/>
-    <mergeCell ref="EL1:EO1"/>
-    <mergeCell ref="EP1:ES1"/>
-    <mergeCell ref="ET1:EW1"/>
-    <mergeCell ref="EX1:FA1"/>
-    <mergeCell ref="FB1:FE1"/>
-    <mergeCell ref="FF1:FI1"/>
-    <mergeCell ref="FJ1:FM1"/>
-    <mergeCell ref="FN1:FQ1"/>
-    <mergeCell ref="FR1:FU1"/>
-    <mergeCell ref="FV1:FY1"/>
-    <mergeCell ref="FZ1:GC1"/>
-    <mergeCell ref="GD1:GG1"/>
-    <mergeCell ref="GH1:GK1"/>
-    <mergeCell ref="GL1:GO1"/>
-    <mergeCell ref="GP1:GS1"/>
-    <mergeCell ref="GT1:GW1"/>
-    <mergeCell ref="GX1:HA1"/>
-    <mergeCell ref="HB1:HE1"/>
-    <mergeCell ref="HF1:HI1"/>
-    <mergeCell ref="HJ1:HM1"/>
-    <mergeCell ref="HN1:HQ1"/>
-    <mergeCell ref="HR1:HU1"/>
-    <mergeCell ref="HV1:HY1"/>
-    <mergeCell ref="HZ1:IC1"/>
-    <mergeCell ref="ID1:IG1"/>
-    <mergeCell ref="IH1:IK1"/>
-    <mergeCell ref="IL1:IO1"/>
+    <mergeCell ref="J1:N1"/>
+    <mergeCell ref="O1:S1"/>
+    <mergeCell ref="T1:X1"/>
+    <mergeCell ref="Y1:AC1"/>
+    <mergeCell ref="AD1:AH1"/>
+    <mergeCell ref="AI1:AM1"/>
+    <mergeCell ref="AN1:AR1"/>
+    <mergeCell ref="AS1:AW1"/>
+    <mergeCell ref="AX1:BB1"/>
+    <mergeCell ref="BC1:BG1"/>
+    <mergeCell ref="BH1:BL1"/>
+    <mergeCell ref="BM1:BQ1"/>
+    <mergeCell ref="BR1:BV1"/>
+    <mergeCell ref="BW1:CA1"/>
+    <mergeCell ref="CB1:CF1"/>
+    <mergeCell ref="CG1:CK1"/>
+    <mergeCell ref="CL1:CP1"/>
+    <mergeCell ref="CQ1:CU1"/>
+    <mergeCell ref="CV1:CZ1"/>
+    <mergeCell ref="DA1:DE1"/>
+    <mergeCell ref="DF1:DJ1"/>
+    <mergeCell ref="DK1:DO1"/>
+    <mergeCell ref="DP1:DT1"/>
+    <mergeCell ref="DU1:DY1"/>
+    <mergeCell ref="DZ1:ED1"/>
+    <mergeCell ref="EE1:EI1"/>
+    <mergeCell ref="EJ1:EN1"/>
+    <mergeCell ref="EO1:ES1"/>
+    <mergeCell ref="ET1:EX1"/>
+    <mergeCell ref="EY1:FC1"/>
+    <mergeCell ref="FD1:FH1"/>
+    <mergeCell ref="FI1:FM1"/>
+    <mergeCell ref="FN1:FR1"/>
+    <mergeCell ref="FS1:FW1"/>
+    <mergeCell ref="FX1:GB1"/>
+    <mergeCell ref="GC1:GG1"/>
+    <mergeCell ref="GH1:GL1"/>
+    <mergeCell ref="GM1:GQ1"/>
+    <mergeCell ref="GR1:GV1"/>
+    <mergeCell ref="GW1:HA1"/>
+    <mergeCell ref="HB1:HF1"/>
+    <mergeCell ref="HG1:HK1"/>
+    <mergeCell ref="HL1:HP1"/>
+    <mergeCell ref="HQ1:HU1"/>
+    <mergeCell ref="HV1:HZ1"/>
+    <mergeCell ref="IA1:IE1"/>
+    <mergeCell ref="IF1:IJ1"/>
+    <mergeCell ref="IK1:IO1"/>
+    <mergeCell ref="IP1:IT1"/>
+    <mergeCell ref="IU1:IY1"/>
+    <mergeCell ref="IZ1:JD1"/>
+    <mergeCell ref="JE1:JI1"/>
+    <mergeCell ref="JJ1:JN1"/>
+    <mergeCell ref="JO1:JS1"/>
+    <mergeCell ref="JT1:JX1"/>
+    <mergeCell ref="JY1:KC1"/>
+    <mergeCell ref="KD1:KH1"/>
+    <mergeCell ref="KI1:KM1"/>
+    <mergeCell ref="KN1:KR1"/>
+    <mergeCell ref="KS1:KW1"/>
   </mergeCells>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>

</xml_diff>